<commit_message>
[Anmol Singh]Interface implemented successfully
</commit_message>
<xml_diff>
--- a/Car_Rental_System.xlsx
+++ b/Car_Rental_System.xlsx
@@ -170,7 +170,7 @@
     <t>Me_AnmolSingh</t>
   </si>
   <si>
-    <t>rTZwfRvKM9clOeAq1tp2c8847Q1cfmt0mSFBdZnHzEQ=</t>
+    <t>l+BDBpDhP3PWK4Fdk1V0gkk7jaTT7MYGlNeda1DFmjs=</t>
   </si>
   <si>
     <t>ghtutgd</t>
@@ -200,7 +200,7 @@
     <t>Me_AmanKaur</t>
   </si>
   <si>
-    <t>1l4TzsMomW/QSE44zyWlZDdjPwvLz4SkxMt9HWle6Vc=</t>
+    <t>JHR8RykEfHhWuFvr2qFg7UOH0poHNV6epBwsNfMvbos=</t>
   </si>
   <si>
     <t>458954hgtfr</t>
@@ -227,7 +227,7 @@
     <t>Me_inshant</t>
   </si>
   <si>
-    <t>gTrcFpVZ6V4wW1ItbHkbjtNsgZfq+asN/fnTZYF57lI=</t>
+    <t>Nc2LEU0rxCIZcxOFSLpqvpvrbnIkyc00SP+VtvQBB3k=</t>
   </si>
   <si>
     <t>inshant</t>
@@ -251,7 +251,7 @@
     <t>Me_Monica</t>
   </si>
   <si>
-    <t>eRd9XSXcJPcVizbPAmOakhCib07+wrhMVlke3eMJ9SE=</t>
+    <t>sl3p02JrjNPZgMMxG3UeO0JJN2tkTf7kpiVVewyoxbU=</t>
   </si>
   <si>
     <t>5485lkjhy</t>
@@ -278,7 +278,7 @@
     <t>Ikroop_Virk</t>
   </si>
   <si>
-    <t>/xgN+g1VqBJGgZJR7c96Em3EsTgNnkAPXsA08He+uLE=</t>
+    <t>B115B8/yKg64ryK4ohFmNI6rR3hGcmHJCR6jWRG2b5k=</t>
   </si>
   <si>
     <t>virkikroop</t>
@@ -299,7 +299,7 @@
     <t>Me_kritima</t>
   </si>
   <si>
-    <t>wpLdl86lGBbyHJZ85LdHN30Oacyxs4fz76xYz/9IOrI=</t>
+    <t>2ExNQn0Sq8qtQa7hbNPPx9yqg8t56+7xl0FzmHdf8PE=</t>
   </si>
   <si>
     <t>5475lkmnj</t>
@@ -314,7 +314,7 @@
     <t>Me_param</t>
   </si>
   <si>
-    <t>IhknhOLSrgTjzAzIgFIkPbzdLUkd5CeRXzsf4We/VjM=</t>
+    <t>V8bBwkyyhFfzJr4tq55HNNxe7usmX7P1VUF7OkRe+TM=</t>
   </si>
   <si>
     <t>paramkaur</t>
@@ -338,7 +338,7 @@
     <t>KumarShanu</t>
   </si>
   <si>
-    <t>RrWp2JpnJCofOVnUlesuKG/NejiGNfbdalcqbqt8ikM=</t>
+    <t>xvPROODH23AWNs6tXxgQ98YaMoqyYdjCFo5+YUSrpfs=</t>
   </si>
   <si>
     <t>kjhujh</t>
@@ -347,16 +347,16 @@
     <t>Clear</t>
   </si>
   <si>
-    <t>o5g1X1mBDSADOdrOmQinitFO2MOFlURiGgEfgaZk/VM=</t>
-  </si>
-  <si>
-    <t>PY4yf4KWTRmWy+YFiWYoVQOmACGu7ozNmXfRWKnuriI=</t>
-  </si>
-  <si>
-    <t>dy1EpaSVrgyt64d25WTE6N9kTEKBK4tkwibPcSFLuNo=</t>
-  </si>
-  <si>
-    <t>qV9lXWM8KH0ONNJIs+0RwSe2gHR2WgdstVWEcgMV298=</t>
+    <t>xPCZJISMu3W5wCYgS4zrOB1nY03UzSGYcJcyNhg9o2w=</t>
+  </si>
+  <si>
+    <t>erlEc/fLo3OLNwoVdIfqtocMPMSjU37j5M5Kvpg8h6g=</t>
+  </si>
+  <si>
+    <t>TO2sBnBGPCnXowSmxLH/nrmKaIMkP5Wkd+8JRP1v2+s=</t>
+  </si>
+  <si>
+    <t>caumWCZ3K+hwiBDrN7Q0P+9yL/qKgfNRqFO8fenzv2o=</t>
   </si>
   <si>
     <t>Caria</t>
@@ -368,7 +368,7 @@
     <t>6723367</t>
   </si>
   <si>
-    <t>yEqlyw2bT9ShTePif3Nwkw9b6lQU6wvUpnKahr8+XS8=</t>
+    <t>F9iYinmeDhDQSVn6dxrCoVUscg122nS/fDmYP0DW25I=</t>
   </si>
   <si>
     <t>ghat</t>
@@ -383,10 +383,10 @@
     <t>auda.org.au</t>
   </si>
   <si>
-    <t>Xf1tcp62ApUFOENtRE03lECjX3JeXdWyglLPKGnvLAI=</t>
-  </si>
-  <si>
-    <t>29/ZRziefdj+KxL4CMAvoKTkvq+UUuKgLXpbabl4g7s=</t>
+    <t>RcQlz8KhXIENPczp0emYjGL2l3o5h0YD48K9WNZuEWI=</t>
+  </si>
+  <si>
+    <t>AisijCSPzx3NL3S7Cmw4tcKGtoAIKIBJ+3hpbL7GAsU=</t>
   </si>
   <si>
     <t>New Car</t>
@@ -500,7 +500,7 @@
     <col min="6" max="6" width="13.96875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="20.828125" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="15.8203125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="50.9921875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="52.140625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="12.28125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="10.59375" customWidth="true" bestFit="true"/>
@@ -558,7 +558,7 @@
         <v>46</v>
       </c>
       <c r="E2" t="n" s="2">
-        <v>28430.63348681713</v>
+        <v>28430.95315505787</v>
       </c>
       <c r="F2" t="s">
         <v>47</v>
@@ -596,7 +596,7 @@
         <v>56</v>
       </c>
       <c r="E3" t="n" s="2">
-        <v>28430.63348681713</v>
+        <v>28430.95315505787</v>
       </c>
       <c r="F3" t="s">
         <v>57</v>
@@ -634,7 +634,7 @@
         <v>46</v>
       </c>
       <c r="E4" t="n" s="2">
-        <v>28430.63348681713</v>
+        <v>28430.95315505787</v>
       </c>
       <c r="F4" t="s">
         <v>66</v>
@@ -672,7 +672,7 @@
         <v>56</v>
       </c>
       <c r="E5" t="n" s="2">
-        <v>28430.63348681713</v>
+        <v>28430.95315505787</v>
       </c>
       <c r="F5" t="s">
         <v>74</v>
@@ -710,7 +710,7 @@
         <v>56</v>
       </c>
       <c r="E6" t="n" s="2">
-        <v>28430.63348681713</v>
+        <v>28430.95315505787</v>
       </c>
       <c r="F6" t="s">
         <v>83</v>
@@ -748,7 +748,7 @@
         <v>56</v>
       </c>
       <c r="E7" t="n" s="2">
-        <v>28430.63348681713</v>
+        <v>28430.95315505787</v>
       </c>
       <c r="F7" t="s">
         <v>90</v>
@@ -786,7 +786,7 @@
         <v>56</v>
       </c>
       <c r="E8" t="n" s="2">
-        <v>28430.63348681713</v>
+        <v>28430.95315505787</v>
       </c>
       <c r="F8" t="s">
         <v>90</v>
@@ -832,7 +832,7 @@
     <col min="7" max="7" width="5.77734375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="18.9296875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="14.23828125" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="53.6875" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="51.87890625" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="20.04296875" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="18.6328125" customWidth="true" bestFit="true"/>
@@ -897,7 +897,7 @@
         <v>46</v>
       </c>
       <c r="E2" t="n" s="2">
-        <v>28430.63348681713</v>
+        <v>28430.95315505787</v>
       </c>
       <c r="F2" t="s">
         <v>103</v>
@@ -941,7 +941,7 @@
         <v>46</v>
       </c>
       <c r="E3" t="n" s="2">
-        <v>28430.63348681713</v>
+        <v>28430.95315505787</v>
       </c>
       <c r="F3" t="s">
         <v>103</v>
@@ -985,7 +985,7 @@
         <v>46</v>
       </c>
       <c r="E4" t="n" s="2">
-        <v>28430.63348681713</v>
+        <v>28430.95315505787</v>
       </c>
       <c r="F4" t="s">
         <v>103</v>
@@ -1029,7 +1029,7 @@
         <v>46</v>
       </c>
       <c r="E5" t="n" s="2">
-        <v>28430.63348681713</v>
+        <v>28430.95315505787</v>
       </c>
       <c r="F5" t="s">
         <v>103</v>
@@ -1073,7 +1073,7 @@
         <v>46</v>
       </c>
       <c r="E6" t="n" s="2">
-        <v>28430.63348681713</v>
+        <v>28430.95315505787</v>
       </c>
       <c r="F6" t="s">
         <v>103</v>
@@ -1125,7 +1125,7 @@
     <col min="7" max="7" width="5.77734375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="13.109375" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="14.23828125" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="50.0" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="50.4765625" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="18.09375" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="17.89453125" customWidth="true" bestFit="true"/>
@@ -1190,7 +1190,7 @@
         <v>56</v>
       </c>
       <c r="E2" t="n" s="2">
-        <v>28430.63348681713</v>
+        <v>28430.95315505787</v>
       </c>
       <c r="F2" t="s">
         <v>115</v>
@@ -1234,7 +1234,7 @@
         <v>56</v>
       </c>
       <c r="E3" t="n" s="2">
-        <v>28430.63348681713</v>
+        <v>28430.95315505787</v>
       </c>
       <c r="F3" t="s">
         <v>115</v>
@@ -1278,7 +1278,7 @@
         <v>56</v>
       </c>
       <c r="E4" t="n" s="2">
-        <v>28430.63348681713</v>
+        <v>28430.95315505787</v>
       </c>
       <c r="F4" t="s">
         <v>115</v>

</xml_diff>

<commit_message>
[Anmol Singh]Interface implements in all classes
</commit_message>
<xml_diff>
--- a/Car_Rental_System.xlsx
+++ b/Car_Rental_System.xlsx
@@ -170,7 +170,7 @@
     <t>Me_AnmolSingh</t>
   </si>
   <si>
-    <t>l+BDBpDhP3PWK4Fdk1V0gkk7jaTT7MYGlNeda1DFmjs=</t>
+    <t>29k5k0C0rcGH3fcDqVCFEMFhsWNrCntUheu2eLSs/hU=</t>
   </si>
   <si>
     <t>ghtutgd</t>
@@ -200,7 +200,7 @@
     <t>Me_AmanKaur</t>
   </si>
   <si>
-    <t>JHR8RykEfHhWuFvr2qFg7UOH0poHNV6epBwsNfMvbos=</t>
+    <t>N/aKBnVkBI6GPiqP6w/1xuXlCw78NgTOWUbZI4WqVkM=</t>
   </si>
   <si>
     <t>458954hgtfr</t>
@@ -227,7 +227,7 @@
     <t>Me_inshant</t>
   </si>
   <si>
-    <t>Nc2LEU0rxCIZcxOFSLpqvpvrbnIkyc00SP+VtvQBB3k=</t>
+    <t>uWj5Jk72Xh0DprjFlAMhbA77L5Dunisg3aFCdGf5pww=</t>
   </si>
   <si>
     <t>inshant</t>
@@ -251,7 +251,7 @@
     <t>Me_Monica</t>
   </si>
   <si>
-    <t>sl3p02JrjNPZgMMxG3UeO0JJN2tkTf7kpiVVewyoxbU=</t>
+    <t>S0zNufK4i2mf+hQ9yadrX1W3bE0Qu8sZpSFiubOLzuc=</t>
   </si>
   <si>
     <t>5485lkjhy</t>
@@ -278,7 +278,7 @@
     <t>Ikroop_Virk</t>
   </si>
   <si>
-    <t>B115B8/yKg64ryK4ohFmNI6rR3hGcmHJCR6jWRG2b5k=</t>
+    <t>DpHYvZr2vgH0z6LEStjANi6OEHd1SfAbiFD6d/MPnRU=</t>
   </si>
   <si>
     <t>virkikroop</t>
@@ -299,7 +299,7 @@
     <t>Me_kritima</t>
   </si>
   <si>
-    <t>2ExNQn0Sq8qtQa7hbNPPx9yqg8t56+7xl0FzmHdf8PE=</t>
+    <t>X2U1uaF/gu0Hfq/m92/wY31rUQwdm9TTx8lhArNKbn8=</t>
   </si>
   <si>
     <t>5475lkmnj</t>
@@ -314,7 +314,7 @@
     <t>Me_param</t>
   </si>
   <si>
-    <t>V8bBwkyyhFfzJr4tq55HNNxe7usmX7P1VUF7OkRe+TM=</t>
+    <t>ASJ6u9M3Ltg5sLpg9eJmaD+P/czKtOBATxfgaZ8onQw=</t>
   </si>
   <si>
     <t>paramkaur</t>
@@ -338,7 +338,7 @@
     <t>KumarShanu</t>
   </si>
   <si>
-    <t>xvPROODH23AWNs6tXxgQ98YaMoqyYdjCFo5+YUSrpfs=</t>
+    <t>1VTZlApWK1DqezxcnW1fT4M+gtSeXhZyfP0MEkjLGd0=</t>
   </si>
   <si>
     <t>kjhujh</t>
@@ -347,16 +347,16 @@
     <t>Clear</t>
   </si>
   <si>
-    <t>xPCZJISMu3W5wCYgS4zrOB1nY03UzSGYcJcyNhg9o2w=</t>
-  </si>
-  <si>
-    <t>erlEc/fLo3OLNwoVdIfqtocMPMSjU37j5M5Kvpg8h6g=</t>
-  </si>
-  <si>
-    <t>TO2sBnBGPCnXowSmxLH/nrmKaIMkP5Wkd+8JRP1v2+s=</t>
-  </si>
-  <si>
-    <t>caumWCZ3K+hwiBDrN7Q0P+9yL/qKgfNRqFO8fenzv2o=</t>
+    <t>OJDmGlfoswwdTvJceIdcVxTJKRrB/YAvZe/6yz9ql7c=</t>
+  </si>
+  <si>
+    <t>IqCkrdI9EwaAB494ALK2vfKkmzssvVZ2Oa+JeCYB/8k=</t>
+  </si>
+  <si>
+    <t>dvfTgm52xqLEaCppWbQkKoSx0462FPNnE47rlxpktSo=</t>
+  </si>
+  <si>
+    <t>gC+akQp0Bi2ll/kAbsIkBLaXiFmmThOcO7q+5TtoXI0=</t>
   </si>
   <si>
     <t>Caria</t>
@@ -368,7 +368,7 @@
     <t>6723367</t>
   </si>
   <si>
-    <t>F9iYinmeDhDQSVn6dxrCoVUscg122nS/fDmYP0DW25I=</t>
+    <t>DbJIZZBP74k7YyDX+v+d1aJxlc0vI4BNNqJClFbXTzA=</t>
   </si>
   <si>
     <t>ghat</t>
@@ -383,10 +383,10 @@
     <t>auda.org.au</t>
   </si>
   <si>
-    <t>RcQlz8KhXIENPczp0emYjGL2l3o5h0YD48K9WNZuEWI=</t>
-  </si>
-  <si>
-    <t>AisijCSPzx3NL3S7Cmw4tcKGtoAIKIBJ+3hpbL7GAsU=</t>
+    <t>XQK9M2z4I45FezKgmpYAdZb42DSBcaxzJQaR/1vsdkQ=</t>
+  </si>
+  <si>
+    <t>6Vzzewqz54/eLvw78kfG79mV0fF3es1ljdOuta5WMzA=</t>
   </si>
   <si>
     <t>New Car</t>
@@ -500,7 +500,7 @@
     <col min="6" max="6" width="13.96875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="20.828125" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="15.8203125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="52.140625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="52.22265625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="12.28125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="10.59375" customWidth="true" bestFit="true"/>
@@ -558,7 +558,7 @@
         <v>46</v>
       </c>
       <c r="E2" t="n" s="2">
-        <v>28430.95315505787</v>
+        <v>28430.958761064816</v>
       </c>
       <c r="F2" t="s">
         <v>47</v>
@@ -596,7 +596,7 @@
         <v>56</v>
       </c>
       <c r="E3" t="n" s="2">
-        <v>28430.95315505787</v>
+        <v>28430.958761064816</v>
       </c>
       <c r="F3" t="s">
         <v>57</v>
@@ -634,7 +634,7 @@
         <v>46</v>
       </c>
       <c r="E4" t="n" s="2">
-        <v>28430.95315505787</v>
+        <v>28430.958761064816</v>
       </c>
       <c r="F4" t="s">
         <v>66</v>
@@ -672,7 +672,7 @@
         <v>56</v>
       </c>
       <c r="E5" t="n" s="2">
-        <v>28430.95315505787</v>
+        <v>28430.958761064816</v>
       </c>
       <c r="F5" t="s">
         <v>74</v>
@@ -710,7 +710,7 @@
         <v>56</v>
       </c>
       <c r="E6" t="n" s="2">
-        <v>28430.95315505787</v>
+        <v>28430.958761064816</v>
       </c>
       <c r="F6" t="s">
         <v>83</v>
@@ -748,7 +748,7 @@
         <v>56</v>
       </c>
       <c r="E7" t="n" s="2">
-        <v>28430.95315505787</v>
+        <v>28430.958761064816</v>
       </c>
       <c r="F7" t="s">
         <v>90</v>
@@ -786,7 +786,7 @@
         <v>56</v>
       </c>
       <c r="E8" t="n" s="2">
-        <v>28430.95315505787</v>
+        <v>28430.958761064816</v>
       </c>
       <c r="F8" t="s">
         <v>90</v>
@@ -832,7 +832,7 @@
     <col min="7" max="7" width="5.77734375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="18.9296875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="14.23828125" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="51.87890625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="50.35546875" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="20.04296875" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="18.6328125" customWidth="true" bestFit="true"/>
@@ -897,7 +897,7 @@
         <v>46</v>
       </c>
       <c r="E2" t="n" s="2">
-        <v>28430.95315505787</v>
+        <v>28430.958761064816</v>
       </c>
       <c r="F2" t="s">
         <v>103</v>
@@ -941,7 +941,7 @@
         <v>46</v>
       </c>
       <c r="E3" t="n" s="2">
-        <v>28430.95315505787</v>
+        <v>28430.958761064816</v>
       </c>
       <c r="F3" t="s">
         <v>103</v>
@@ -985,7 +985,7 @@
         <v>46</v>
       </c>
       <c r="E4" t="n" s="2">
-        <v>28430.95315505787</v>
+        <v>28430.958761064816</v>
       </c>
       <c r="F4" t="s">
         <v>103</v>
@@ -1029,7 +1029,7 @@
         <v>46</v>
       </c>
       <c r="E5" t="n" s="2">
-        <v>28430.95315505787</v>
+        <v>28430.958761064816</v>
       </c>
       <c r="F5" t="s">
         <v>103</v>
@@ -1073,7 +1073,7 @@
         <v>46</v>
       </c>
       <c r="E6" t="n" s="2">
-        <v>28430.95315505787</v>
+        <v>28430.958761064816</v>
       </c>
       <c r="F6" t="s">
         <v>103</v>
@@ -1125,7 +1125,7 @@
     <col min="7" max="7" width="5.77734375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="13.109375" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="14.23828125" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="50.4765625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="50.01171875" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="18.09375" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="17.89453125" customWidth="true" bestFit="true"/>
@@ -1190,7 +1190,7 @@
         <v>56</v>
       </c>
       <c r="E2" t="n" s="2">
-        <v>28430.95315505787</v>
+        <v>28430.958761064816</v>
       </c>
       <c r="F2" t="s">
         <v>115</v>
@@ -1234,7 +1234,7 @@
         <v>56</v>
       </c>
       <c r="E3" t="n" s="2">
-        <v>28430.95315505787</v>
+        <v>28430.958761064816</v>
       </c>
       <c r="F3" t="s">
         <v>115</v>
@@ -1278,7 +1278,7 @@
         <v>56</v>
       </c>
       <c r="E4" t="n" s="2">
-        <v>28430.95315505787</v>
+        <v>28430.958761064816</v>
       </c>
       <c r="F4" t="s">
         <v>115</v>

</xml_diff>

<commit_message>
[Anmol Singh]Class ExcelWriter-Data Entry
</commit_message>
<xml_diff>
--- a/Car_Rental_System.xlsx
+++ b/Car_Rental_System.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="182">
   <si>
     <t>ID</t>
   </si>
@@ -170,7 +170,7 @@
     <t>Me_AnmolSingh</t>
   </si>
   <si>
-    <t>29k5k0C0rcGH3fcDqVCFEMFhsWNrCntUheu2eLSs/hU=</t>
+    <t>SnxKNGCq8JgXPZvFSPM1bggA1VouVp4j6Y2OUpAHKWo=</t>
   </si>
   <si>
     <t>ghtutgd</t>
@@ -200,7 +200,7 @@
     <t>Me_AmanKaur</t>
   </si>
   <si>
-    <t>N/aKBnVkBI6GPiqP6w/1xuXlCw78NgTOWUbZI4WqVkM=</t>
+    <t>uHwB0nmUUtjAS5c6HnbgIly3OFQUItBvFVMKnDZ3Cm4=</t>
   </si>
   <si>
     <t>458954hgtfr</t>
@@ -227,7 +227,7 @@
     <t>Me_inshant</t>
   </si>
   <si>
-    <t>uWj5Jk72Xh0DprjFlAMhbA77L5Dunisg3aFCdGf5pww=</t>
+    <t>Sb0CDSHe6xZAPxZ5d0LJH1tJA5Yv3zlvSqt2NTbYqoI=</t>
   </si>
   <si>
     <t>inshant</t>
@@ -251,7 +251,7 @@
     <t>Me_Monica</t>
   </si>
   <si>
-    <t>S0zNufK4i2mf+hQ9yadrX1W3bE0Qu8sZpSFiubOLzuc=</t>
+    <t>mdj1R+osfmwen1QrWVCN5FzarMxapfo1Z3aY7yiwQp4=</t>
   </si>
   <si>
     <t>5485lkjhy</t>
@@ -278,7 +278,7 @@
     <t>Ikroop_Virk</t>
   </si>
   <si>
-    <t>DpHYvZr2vgH0z6LEStjANi6OEHd1SfAbiFD6d/MPnRU=</t>
+    <t>d8o7lo0kydQRzc7VzVFnQFncccuohIEd5ng2rhzY0g4=</t>
   </si>
   <si>
     <t>virkikroop</t>
@@ -299,7 +299,7 @@
     <t>Me_kritima</t>
   </si>
   <si>
-    <t>X2U1uaF/gu0Hfq/m92/wY31rUQwdm9TTx8lhArNKbn8=</t>
+    <t>YAftqNr/sknwNvWPLS34pvNa1XZL42lQ/qqqJe0Oi7c=</t>
   </si>
   <si>
     <t>5475lkmnj</t>
@@ -314,7 +314,7 @@
     <t>Me_param</t>
   </si>
   <si>
-    <t>ASJ6u9M3Ltg5sLpg9eJmaD+P/czKtOBATxfgaZ8onQw=</t>
+    <t>3MUD/qzBk1sr/PqQnIo5yeWTPad0n38BlarkQbR12hA=</t>
   </si>
   <si>
     <t>paramkaur</t>
@@ -338,7 +338,7 @@
     <t>KumarShanu</t>
   </si>
   <si>
-    <t>1VTZlApWK1DqezxcnW1fT4M+gtSeXhZyfP0MEkjLGd0=</t>
+    <t>971jNt/If8odXoWVszPjEfUSQr8r1H11MaegceZxMVc=</t>
   </si>
   <si>
     <t>kjhujh</t>
@@ -347,16 +347,106 @@
     <t>Clear</t>
   </si>
   <si>
-    <t>OJDmGlfoswwdTvJceIdcVxTJKRrB/YAvZe/6yz9ql7c=</t>
-  </si>
-  <si>
-    <t>IqCkrdI9EwaAB494ALK2vfKkmzssvVZ2Oa+JeCYB/8k=</t>
-  </si>
-  <si>
-    <t>dvfTgm52xqLEaCppWbQkKoSx0462FPNnE47rlxpktSo=</t>
-  </si>
-  <si>
-    <t>gC+akQp0Bi2ll/kAbsIkBLaXiFmmThOcO7q+5TtoXI0=</t>
+    <t>$5445.0</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>6544875984</t>
+  </si>
+  <si>
+    <t>micheal@jordan.com</t>
+  </si>
+  <si>
+    <t>Jordan_Micheal</t>
+  </si>
+  <si>
+    <t>uS7Nwf3uty3qobw8QAspC4NxTab5b66eQykDivlXUdA=</t>
+  </si>
+  <si>
+    <t>dfgtre3</t>
+  </si>
+  <si>
+    <t>Unclear</t>
+  </si>
+  <si>
+    <t>$2045.1500244140625</t>
+  </si>
+  <si>
+    <t>Michelle</t>
+  </si>
+  <si>
+    <t>Rai</t>
+  </si>
+  <si>
+    <t>8547256318</t>
+  </si>
+  <si>
+    <t>michelle@gmail.com</t>
+  </si>
+  <si>
+    <t>michelle</t>
+  </si>
+  <si>
+    <t>s4rKF7xE8h7LsKVjczS8FUvwbeJBnsaagTj58QxQHSo=</t>
+  </si>
+  <si>
+    <t>1254gytr</t>
+  </si>
+  <si>
+    <t>$1145.050048828125</t>
+  </si>
+  <si>
+    <t>Sherin</t>
+  </si>
+  <si>
+    <t>Gupta</t>
+  </si>
+  <si>
+    <t>98564748572</t>
+  </si>
+  <si>
+    <t>gupSherin@yahoo.com</t>
+  </si>
+  <si>
+    <t>SherinG</t>
+  </si>
+  <si>
+    <t>o+9qO3keitE8h8kTOYntdFYxgQz2AUsjohefVynGxBM=</t>
+  </si>
+  <si>
+    <t>524plo;</t>
+  </si>
+  <si>
+    <t>$998.4000244140625</t>
+  </si>
+  <si>
+    <t>Rakesh</t>
+  </si>
+  <si>
+    <t>Jain</t>
+  </si>
+  <si>
+    <t>9852395452</t>
+  </si>
+  <si>
+    <t>jainbhai@gmail.com</t>
+  </si>
+  <si>
+    <t>JainSaab</t>
+  </si>
+  <si>
+    <t>lAsQq2vfAIe95eK1MygxfhOhGgYSbrn5kpszgFvnmvg=</t>
+  </si>
+  <si>
+    <t>ppo;;lko</t>
+  </si>
+  <si>
+    <t>$840.1500244140625</t>
   </si>
   <si>
     <t>Caria</t>
@@ -365,10 +455,10 @@
     <t>MacNamee</t>
   </si>
   <si>
-    <t>6723367</t>
-  </si>
-  <si>
-    <t>DbJIZZBP74k7YyDX+v+d1aJxlc0vI4BNNqJClFbXTzA=</t>
+    <t>6723367567</t>
+  </si>
+  <si>
+    <t>/nOYo/0oZu97hS18lhJZMYzLWEeJFy2JSE+n5y0RoSg=</t>
   </si>
   <si>
     <t>ghat</t>
@@ -383,10 +473,58 @@
     <t>auda.org.au</t>
   </si>
   <si>
-    <t>XQK9M2z4I45FezKgmpYAdZb42DSBcaxzJQaR/1vsdkQ=</t>
-  </si>
-  <si>
-    <t>6Vzzewqz54/eLvw78kfG79mV0fF3es1ljdOuta5WMzA=</t>
+    <t>Gillingum</t>
+  </si>
+  <si>
+    <t>Road</t>
+  </si>
+  <si>
+    <t>6892145763</t>
+  </si>
+  <si>
+    <t>gillingum@gillingum.com</t>
+  </si>
+  <si>
+    <t>qdH92Laeqmdy5HbGIYKF1TCdqUGcGnycJnwH0JlJ2o8=</t>
+  </si>
+  <si>
+    <t>dhobi_ghat</t>
+  </si>
+  <si>
+    <t>Officials</t>
+  </si>
+  <si>
+    <t>2471596587</t>
+  </si>
+  <si>
+    <t>officials.org.au</t>
+  </si>
+  <si>
+    <t>Careem</t>
+  </si>
+  <si>
+    <t>Nazi</t>
+  </si>
+  <si>
+    <t>9988456321</t>
+  </si>
+  <si>
+    <t>careem@me.com</t>
+  </si>
+  <si>
+    <t>Dv1xXTNC5IO+v3NZMCsUzNT3GhcoqW7HLR40LPJcCdE=</t>
+  </si>
+  <si>
+    <t>Gaziattack</t>
+  </si>
+  <si>
+    <t>DCompany</t>
+  </si>
+  <si>
+    <t>2985421526</t>
+  </si>
+  <si>
+    <t>ComapnyD.org.au</t>
   </si>
   <si>
     <t>New Car</t>
@@ -500,7 +638,7 @@
     <col min="6" max="6" width="13.96875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="20.828125" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="15.8203125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="52.22265625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="52.29296875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="12.28125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="10.59375" customWidth="true" bestFit="true"/>
@@ -558,7 +696,7 @@
         <v>46</v>
       </c>
       <c r="E2" t="n" s="2">
-        <v>28430.958761064816</v>
+        <v>28430.030026724537</v>
       </c>
       <c r="F2" t="s">
         <v>47</v>
@@ -596,7 +734,7 @@
         <v>56</v>
       </c>
       <c r="E3" t="n" s="2">
-        <v>28430.958761064816</v>
+        <v>28430.030026724537</v>
       </c>
       <c r="F3" t="s">
         <v>57</v>
@@ -634,7 +772,7 @@
         <v>46</v>
       </c>
       <c r="E4" t="n" s="2">
-        <v>28430.958761064816</v>
+        <v>28430.030026724537</v>
       </c>
       <c r="F4" t="s">
         <v>66</v>
@@ -672,7 +810,7 @@
         <v>56</v>
       </c>
       <c r="E5" t="n" s="2">
-        <v>28430.958761064816</v>
+        <v>28430.030026724537</v>
       </c>
       <c r="F5" t="s">
         <v>74</v>
@@ -710,7 +848,7 @@
         <v>56</v>
       </c>
       <c r="E6" t="n" s="2">
-        <v>28430.958761064816</v>
+        <v>28430.030026724537</v>
       </c>
       <c r="F6" t="s">
         <v>83</v>
@@ -748,7 +886,7 @@
         <v>56</v>
       </c>
       <c r="E7" t="n" s="2">
-        <v>28430.958761064816</v>
+        <v>28430.030026724537</v>
       </c>
       <c r="F7" t="s">
         <v>90</v>
@@ -786,7 +924,7 @@
         <v>56</v>
       </c>
       <c r="E8" t="n" s="2">
-        <v>28430.958761064816</v>
+        <v>28430.030026724537</v>
       </c>
       <c r="F8" t="s">
         <v>90</v>
@@ -830,13 +968,13 @@
     <col min="5" max="5" width="11.3046875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="13.96875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="5.77734375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="18.9296875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="14.23828125" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="50.35546875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="21.96875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="15.25" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="50.48046875" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="20.04296875" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="18.6328125" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="12.7421875" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="21.66015625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -885,7 +1023,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>11265.0</v>
+        <v>12265.0</v>
       </c>
       <c r="B2" t="s">
         <v>101</v>
@@ -897,7 +1035,7 @@
         <v>46</v>
       </c>
       <c r="E2" t="n" s="2">
-        <v>28430.958761064816</v>
+        <v>28430.030026724537</v>
       </c>
       <c r="F2" t="s">
         <v>103</v>
@@ -923,184 +1061,184 @@
       <c r="M2" t="s">
         <v>108</v>
       </c>
-      <c r="N2" t="n">
-        <v>5445.0</v>
+      <c r="N2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>11265.0</v>
+        <v>12271.0</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="C3" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="D3" t="s">
         <v>46</v>
       </c>
       <c r="E3" t="n" s="2">
-        <v>28430.958761064816</v>
+        <v>28430.030026724537</v>
       </c>
       <c r="F3" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="G3" t="n">
         <v>0.0</v>
       </c>
       <c r="H3" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="I3" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="J3" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="K3" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="L3" t="n">
-        <v>456854.0</v>
+        <v>854787.0</v>
       </c>
       <c r="M3" t="s">
-        <v>108</v>
-      </c>
-      <c r="N3" t="n">
-        <v>5445.0</v>
+        <v>117</v>
+      </c>
+      <c r="N3" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>11265.0</v>
+        <v>12236.0</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="E4" t="n" s="2">
-        <v>28430.958761064816</v>
+        <v>28430.030026724537</v>
       </c>
       <c r="F4" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="G4" t="n">
         <v>0.0</v>
       </c>
       <c r="H4" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="I4" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="J4" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="K4" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="L4" t="n">
-        <v>456854.0</v>
+        <v>169754.0</v>
       </c>
       <c r="M4" t="s">
-        <v>108</v>
-      </c>
-      <c r="N4" t="n">
-        <v>5445.0</v>
+        <v>117</v>
+      </c>
+      <c r="N4" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>11265.0</v>
+        <v>12451.0</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
+        <v>127</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>128</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="E5" t="n" s="2">
-        <v>28430.958761064816</v>
+        <v>28430.030026724537</v>
       </c>
       <c r="F5" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="G5" t="n">
         <v>0.0</v>
       </c>
       <c r="H5" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="I5" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="J5" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="K5" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
       <c r="L5" t="n">
-        <v>456854.0</v>
+        <v>233256.0</v>
       </c>
       <c r="M5" t="s">
         <v>108</v>
       </c>
-      <c r="N5" t="n">
-        <v>5445.0</v>
+      <c r="N5" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>11265.0</v>
+        <v>12781.0</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>135</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>136</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
       </c>
       <c r="E6" t="n" s="2">
-        <v>28430.958761064816</v>
+        <v>28430.030026724537</v>
       </c>
       <c r="F6" t="s">
-        <v>103</v>
+        <v>137</v>
       </c>
       <c r="G6" t="n">
         <v>0.0</v>
       </c>
       <c r="H6" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
       <c r="I6" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="J6" t="s">
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="K6" t="s">
-        <v>107</v>
+        <v>141</v>
       </c>
       <c r="L6" t="n">
-        <v>456854.0</v>
+        <v>115897.0</v>
       </c>
       <c r="M6" t="s">
         <v>108</v>
       </c>
-      <c r="N6" t="n">
-        <v>540.1500244140625</v>
+      <c r="N6" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1110,26 +1248,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="4.37890625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="6.609375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="13.9453125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="13.54296875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="9.9453125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="11.3046875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="13.96875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="5.77734375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="13.109375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="14.23828125" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="50.01171875" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="22.3359375" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="18.09375" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="17.89453125" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="11.73828125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="23.7265625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="14.23828125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="51.61328125" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="22.3359375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="18.09375" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="17.89453125" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="17.125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1152,160 +1289,148 @@
         <v>5</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>17</v>
-      </c>
-      <c r="N1" t="s" s="1">
         <v>18</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>111.0</v>
+        <v>13981.0</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>143</v>
       </c>
       <c r="C2" t="s">
-        <v>114</v>
+        <v>144</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
       </c>
       <c r="E2" t="n" s="2">
-        <v>28430.958761064816</v>
+        <v>28430.030026724537</v>
       </c>
       <c r="F2" t="s">
-        <v>115</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.0</v>
+        <v>145</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
       </c>
       <c r="H2" t="s">
-        <v>48</v>
+        <v>143</v>
       </c>
       <c r="I2" t="s">
-        <v>113</v>
+        <v>146</v>
       </c>
       <c r="J2" t="s">
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="K2" t="s">
-        <v>117</v>
+        <v>148</v>
       </c>
       <c r="L2" t="s">
-        <v>118</v>
+        <v>149</v>
       </c>
       <c r="M2" t="s">
-        <v>119</v>
-      </c>
-      <c r="N2" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>111.0</v>
+        <v>13657.0</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>151</v>
       </c>
       <c r="C3" t="s">
-        <v>114</v>
+        <v>152</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E3" t="n" s="2">
-        <v>28430.958761064816</v>
+        <v>28430.030026724537</v>
       </c>
       <c r="F3" t="s">
-        <v>115</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.0</v>
+        <v>153</v>
+      </c>
+      <c r="G3" t="s">
+        <v>154</v>
       </c>
       <c r="H3" t="s">
-        <v>48</v>
+        <v>152</v>
       </c>
       <c r="I3" t="s">
-        <v>113</v>
+        <v>155</v>
       </c>
       <c r="J3" t="s">
-        <v>121</v>
+        <v>156</v>
       </c>
       <c r="K3" t="s">
-        <v>117</v>
+        <v>157</v>
       </c>
       <c r="L3" t="s">
-        <v>118</v>
+        <v>158</v>
       </c>
       <c r="M3" t="s">
-        <v>119</v>
-      </c>
-      <c r="N3" t="s">
-        <v>120</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>111.0</v>
+        <v>13215.0</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>160</v>
       </c>
       <c r="C4" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="D4" t="s">
         <v>56</v>
       </c>
       <c r="E4" t="n" s="2">
-        <v>28430.958761064816</v>
+        <v>28430.030026724537</v>
       </c>
       <c r="F4" t="s">
-        <v>115</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.0</v>
+        <v>162</v>
+      </c>
+      <c r="G4" t="s">
+        <v>163</v>
       </c>
       <c r="H4" t="s">
-        <v>48</v>
+        <v>160</v>
       </c>
       <c r="I4" t="s">
-        <v>113</v>
+        <v>164</v>
       </c>
       <c r="J4" t="s">
-        <v>122</v>
+        <v>165</v>
       </c>
       <c r="K4" t="s">
-        <v>117</v>
+        <v>166</v>
       </c>
       <c r="L4" t="s">
-        <v>118</v>
+        <v>167</v>
       </c>
       <c r="M4" t="s">
-        <v>119</v>
-      </c>
-      <c r="N4" t="s">
-        <v>120</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -1382,10 +1507,10 @@
         <v>11254.0</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>169</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>170</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1399,7 +1524,7 @@
         <v>4.0</v>
       </c>
       <c r="I2" t="s">
-        <v>125</v>
+        <v>171</v>
       </c>
       <c r="J2" t="n">
         <v>250.0</v>
@@ -1408,10 +1533,10 @@
         <v>7.0</v>
       </c>
       <c r="L2" t="s">
-        <v>126</v>
+        <v>172</v>
       </c>
       <c r="M2" t="s">
-        <v>127</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3">
@@ -1419,10 +1544,10 @@
         <v>11254.0</v>
       </c>
       <c r="B3" t="s">
-        <v>123</v>
+        <v>169</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>170</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
@@ -1436,7 +1561,7 @@
         <v>4.0</v>
       </c>
       <c r="I3" t="s">
-        <v>125</v>
+        <v>171</v>
       </c>
       <c r="J3" t="n">
         <v>250.0</v>
@@ -1445,10 +1570,10 @@
         <v>7.0</v>
       </c>
       <c r="L3" t="s">
-        <v>126</v>
+        <v>172</v>
       </c>
       <c r="M3" t="s">
-        <v>127</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4">
@@ -1456,10 +1581,10 @@
         <v>11254.0</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>169</v>
       </c>
       <c r="C4" t="s">
-        <v>124</v>
+        <v>170</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -1473,7 +1598,7 @@
         <v>4.0</v>
       </c>
       <c r="I4" t="s">
-        <v>125</v>
+        <v>171</v>
       </c>
       <c r="J4" t="n">
         <v>250.0</v>
@@ -1482,10 +1607,10 @@
         <v>7.0</v>
       </c>
       <c r="L4" t="s">
-        <v>126</v>
+        <v>172</v>
       </c>
       <c r="M4" t="s">
-        <v>127</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -1509,7 +1634,7 @@
     <col min="6" max="6" width="11.921875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="30.76171875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="15.09375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="6.4375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="7.578125" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="12.79296875" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="15.6640625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="13.515625" customWidth="true" bestFit="true"/>
@@ -1562,10 +1687,10 @@
         <v>11254.0</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>174</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>170</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1579,7 +1704,7 @@
         <v>2.0</v>
       </c>
       <c r="I2" t="s">
-        <v>129</v>
+        <v>175</v>
       </c>
       <c r="J2" t="n">
         <v>250.0</v>
@@ -1599,10 +1724,10 @@
         <v>11254.0</v>
       </c>
       <c r="B3" t="s">
-        <v>128</v>
+        <v>174</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>170</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
@@ -1616,7 +1741,7 @@
         <v>2.0</v>
       </c>
       <c r="I3" t="s">
-        <v>129</v>
+        <v>175</v>
       </c>
       <c r="J3" t="n">
         <v>250.0</v>
@@ -1636,10 +1761,10 @@
         <v>11254.0</v>
       </c>
       <c r="B4" t="s">
-        <v>128</v>
+        <v>174</v>
       </c>
       <c r="C4" t="s">
-        <v>124</v>
+        <v>170</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -1653,7 +1778,7 @@
         <v>2.0</v>
       </c>
       <c r="I4" t="s">
-        <v>129</v>
+        <v>171</v>
       </c>
       <c r="J4" t="n">
         <v>250.0</v>
@@ -1746,10 +1871,10 @@
         <v>11254.0</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>176</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>170</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1763,7 +1888,7 @@
         <v>7.0</v>
       </c>
       <c r="I2" t="s">
-        <v>125</v>
+        <v>171</v>
       </c>
       <c r="J2" t="n">
         <v>250.0</v>
@@ -1772,7 +1897,7 @@
         <v>7.0</v>
       </c>
       <c r="L2" t="s">
-        <v>131</v>
+        <v>177</v>
       </c>
       <c r="M2" t="b">
         <v>1</v>
@@ -1786,10 +1911,10 @@
         <v>11254.0</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>176</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>170</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
@@ -1803,7 +1928,7 @@
         <v>7.0</v>
       </c>
       <c r="I3" t="s">
-        <v>125</v>
+        <v>171</v>
       </c>
       <c r="J3" t="n">
         <v>250.0</v>
@@ -1812,7 +1937,7 @@
         <v>7.0</v>
       </c>
       <c r="L3" t="s">
-        <v>131</v>
+        <v>177</v>
       </c>
       <c r="M3" t="b">
         <v>1</v>
@@ -1826,17 +1951,15 @@
         <v>11254.0</v>
       </c>
       <c r="B4" t="s">
-        <v>130</v>
+        <v>176</v>
       </c>
       <c r="C4" t="s">
-        <v>124</v>
+        <v>170</v>
       </c>
       <c r="D4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>44</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E4"/>
       <c r="F4" t="b">
         <v>0</v>
       </c>
@@ -1845,7 +1968,7 @@
         <v>7.0</v>
       </c>
       <c r="I4" t="s">
-        <v>125</v>
+        <v>171</v>
       </c>
       <c r="J4" t="n">
         <v>250.0</v>
@@ -1854,7 +1977,7 @@
         <v>7.0</v>
       </c>
       <c r="L4" t="s">
-        <v>131</v>
+        <v>177</v>
       </c>
       <c r="M4" t="b">
         <v>1</v>
@@ -1910,19 +2033,19 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>178</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>179</v>
       </c>
       <c r="C2" t="n">
         <v>10.0</v>
       </c>
       <c r="D2" t="s">
-        <v>134</v>
+        <v>180</v>
       </c>
       <c r="E2" t="s">
-        <v>135</v>
+        <v>181</v>
       </c>
       <c r="F2" t="n">
         <v>15.25</v>
@@ -1933,19 +2056,19 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>132</v>
+        <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>133</v>
+        <v>179</v>
       </c>
       <c r="C3" t="n">
         <v>10.0</v>
       </c>
       <c r="D3" t="s">
-        <v>134</v>
+        <v>180</v>
       </c>
       <c r="E3" t="s">
-        <v>135</v>
+        <v>181</v>
       </c>
       <c r="F3" t="n">
         <v>15.25</v>
@@ -1956,19 +2079,19 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>178</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>179</v>
       </c>
       <c r="C4" t="n">
         <v>10.0</v>
       </c>
       <c r="D4" t="s">
-        <v>134</v>
+        <v>180</v>
       </c>
       <c r="E4" t="s">
-        <v>135</v>
+        <v>181</v>
       </c>
       <c r="F4" t="n">
         <v>15.25</v>

</xml_diff>

<commit_message>
[Anmol Singh]Class ExcelWriter-Data Duplication error encountered
</commit_message>
<xml_diff>
--- a/Car_Rental_System.xlsx
+++ b/Car_Rental_System.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="217">
   <si>
     <t>ID</t>
   </si>
@@ -170,7 +170,7 @@
     <t>Me_AnmolSingh</t>
   </si>
   <si>
-    <t>SnxKNGCq8JgXPZvFSPM1bggA1VouVp4j6Y2OUpAHKWo=</t>
+    <t>MLsex7I0KUyCAevDbMImc1XBcC+gVvs+jIdPx6nuGCA=</t>
   </si>
   <si>
     <t>ghtutgd</t>
@@ -200,7 +200,7 @@
     <t>Me_AmanKaur</t>
   </si>
   <si>
-    <t>uHwB0nmUUtjAS5c6HnbgIly3OFQUItBvFVMKnDZ3Cm4=</t>
+    <t>uFomyJUvMUbjAE6BpcEixEy0H9/RDJ2ogHuy+awlF1E=</t>
   </si>
   <si>
     <t>458954hgtfr</t>
@@ -227,7 +227,7 @@
     <t>Me_inshant</t>
   </si>
   <si>
-    <t>Sb0CDSHe6xZAPxZ5d0LJH1tJA5Yv3zlvSqt2NTbYqoI=</t>
+    <t>tmKaj15OEV7SG2etsSgEDozGWQqT5JWURm9jLr3lrAY=</t>
   </si>
   <si>
     <t>inshant</t>
@@ -251,7 +251,7 @@
     <t>Me_Monica</t>
   </si>
   <si>
-    <t>mdj1R+osfmwen1QrWVCN5FzarMxapfo1Z3aY7yiwQp4=</t>
+    <t>D1kcEXZRDAH7f7rwj/wan5EPsn2zjKD/4U9hc+i4glU=</t>
   </si>
   <si>
     <t>5485lkjhy</t>
@@ -278,7 +278,7 @@
     <t>Ikroop_Virk</t>
   </si>
   <si>
-    <t>d8o7lo0kydQRzc7VzVFnQFncccuohIEd5ng2rhzY0g4=</t>
+    <t>Oxh7ejzPqvg/rgaXMoCXwZnTiZxcJjJ/eOaHGLwSFdo=</t>
   </si>
   <si>
     <t>virkikroop</t>
@@ -299,7 +299,7 @@
     <t>Me_kritima</t>
   </si>
   <si>
-    <t>YAftqNr/sknwNvWPLS34pvNa1XZL42lQ/qqqJe0Oi7c=</t>
+    <t>AUii3G7lRdxcqfxDmAXWgKY7jIrSe0ba4GpuKd+2cDo=</t>
   </si>
   <si>
     <t>5475lkmnj</t>
@@ -314,7 +314,7 @@
     <t>Me_param</t>
   </si>
   <si>
-    <t>3MUD/qzBk1sr/PqQnIo5yeWTPad0n38BlarkQbR12hA=</t>
+    <t>5f9LzyL1RiEP29LxAIWL51+UCHD9rSVfN8foLcaqBNw=</t>
   </si>
   <si>
     <t>paramkaur</t>
@@ -338,7 +338,7 @@
     <t>KumarShanu</t>
   </si>
   <si>
-    <t>971jNt/If8odXoWVszPjEfUSQr8r1H11MaegceZxMVc=</t>
+    <t>YM46aLrktAM0L2Ijzatm+bPD7ekLyMUBbyFLr7yS7IA=</t>
   </si>
   <si>
     <t>kjhujh</t>
@@ -365,7 +365,7 @@
     <t>Jordan_Micheal</t>
   </si>
   <si>
-    <t>uS7Nwf3uty3qobw8QAspC4NxTab5b66eQykDivlXUdA=</t>
+    <t>4+P61+ueT1J/pZBdZ4CIX+f59mAUqWm94DLbAh+NhJM=</t>
   </si>
   <si>
     <t>dfgtre3</t>
@@ -392,7 +392,7 @@
     <t>michelle</t>
   </si>
   <si>
-    <t>s4rKF7xE8h7LsKVjczS8FUvwbeJBnsaagTj58QxQHSo=</t>
+    <t>QJjyPUmHZ1HyOujHmG/VTzBJg2JLKKn7yaJgo3Ci9x8=</t>
   </si>
   <si>
     <t>1254gytr</t>
@@ -416,7 +416,7 @@
     <t>SherinG</t>
   </si>
   <si>
-    <t>o+9qO3keitE8h8kTOYntdFYxgQz2AUsjohefVynGxBM=</t>
+    <t>jUatMlThD/JbO/2I7Zhc12pqnzP7ni2NSNLZP0yRT0s=</t>
   </si>
   <si>
     <t>524plo;</t>
@@ -440,7 +440,7 @@
     <t>JainSaab</t>
   </si>
   <si>
-    <t>lAsQq2vfAIe95eK1MygxfhOhGgYSbrn5kpszgFvnmvg=</t>
+    <t>jZCWcGTlimZFMZBGAI2sSzvneg716kEjXn59Fc8Qn/4=</t>
   </si>
   <si>
     <t>ppo;;lko</t>
@@ -458,7 +458,7 @@
     <t>6723367567</t>
   </si>
   <si>
-    <t>/nOYo/0oZu97hS18lhJZMYzLWEeJFy2JSE+n5y0RoSg=</t>
+    <t>tk1VQQSYIAyUHCJ729eunNq71X9Id7pEPbwsROPUJ6I=</t>
   </si>
   <si>
     <t>ghat</t>
@@ -485,7 +485,7 @@
     <t>gillingum@gillingum.com</t>
   </si>
   <si>
-    <t>qdH92Laeqmdy5HbGIYKF1TCdqUGcGnycJnwH0JlJ2o8=</t>
+    <t>VKxJ0X+3sFilno3aIXMHvj1MngEsKDMQF5v6XAjGXB4=</t>
   </si>
   <si>
     <t>dhobi_ghat</t>
@@ -512,7 +512,7 @@
     <t>careem@me.com</t>
   </si>
   <si>
-    <t>Dv1xXTNC5IO+v3NZMCsUzNT3GhcoqW7HLR40LPJcCdE=</t>
+    <t>Z79RO7SfLmurq8+Qmv3MiFgD1gbPQWLQkM2E8m1p0gg=</t>
   </si>
   <si>
     <t>Gaziattack</t>
@@ -527,28 +527,130 @@
     <t>ComapnyD.org.au</t>
   </si>
   <si>
-    <t>New Car</t>
+    <t>JHMZF1C67BS073397</t>
+  </si>
+  <si>
+    <t>Mustang</t>
+  </si>
+  <si>
+    <t>Ford</t>
+  </si>
+  <si>
+    <t>IP1</t>
+  </si>
+  <si>
+    <t>Diesel</t>
+  </si>
+  <si>
+    <t>Sport</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>5TBRU34155S423198</t>
+  </si>
+  <si>
+    <t>G-Wagon</t>
+  </si>
+  <si>
+    <t>Mercedes</t>
+  </si>
+  <si>
+    <t>IP5</t>
+  </si>
+  <si>
+    <t>Petrol</t>
+  </si>
+  <si>
+    <t>SUV</t>
+  </si>
+  <si>
+    <t>Space-Grey</t>
+  </si>
+  <si>
+    <t>JTHKD5BH8D2168653</t>
+  </si>
+  <si>
+    <t>Civic</t>
+  </si>
+  <si>
+    <t>Hyundai</t>
+  </si>
+  <si>
+    <t>IP4</t>
+  </si>
+  <si>
+    <t>Electric</t>
+  </si>
+  <si>
+    <t>Sedan</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>1FTSW21RX8EC53647</t>
+  </si>
+  <si>
+    <t>Davidson</t>
+  </si>
+  <si>
+    <t>Harley</t>
+  </si>
+  <si>
+    <t>2HKRL1863YH598774</t>
+  </si>
+  <si>
+    <t>BMX</t>
+  </si>
+  <si>
+    <t>BMW</t>
+  </si>
+  <si>
+    <t>1J4BA6H11AL289387</t>
+  </si>
+  <si>
+    <t>Bullet</t>
+  </si>
+  <si>
+    <t>Royal Enfield</t>
+  </si>
+  <si>
+    <t>5LMCJ1A97FUJ59251</t>
   </si>
   <si>
     <t>Volvo</t>
   </si>
   <si>
-    <t>Electric</t>
-  </si>
-  <si>
-    <t>Sedan</t>
-  </si>
-  <si>
-    <t>Blue</t>
-  </si>
-  <si>
-    <t>Hashtag</t>
-  </si>
-  <si>
-    <t>Petrol</t>
-  </si>
-  <si>
-    <t>Here only</t>
+    <t>BusCompany-A</t>
+  </si>
+  <si>
+    <t>Micheal</t>
+  </si>
+  <si>
+    <t>1G1ZT548X5F147693</t>
+  </si>
+  <si>
+    <t>Double_decker</t>
+  </si>
+  <si>
+    <t>BusCompany-B</t>
+  </si>
+  <si>
+    <t>IP3</t>
+  </si>
+  <si>
+    <t>DoubleDecker</t>
+  </si>
+  <si>
+    <t>SALFR2BG0EH387740</t>
+  </si>
+  <si>
+    <t>Mini_coach</t>
+  </si>
+  <si>
+    <t>BusCompany-C</t>
   </si>
   <si>
     <t>MiniCoach</t>
@@ -560,10 +662,13 @@
     <t>2020-01-25</t>
   </si>
   <si>
-    <t>Harley</t>
-  </si>
-  <si>
     <t>MOTORCYCLE</t>
+  </si>
+  <si>
+    <t>2020-02-20</t>
+  </si>
+  <si>
+    <t>Invalid Vehicle Entry</t>
   </si>
 </sst>
 </file>
@@ -638,7 +743,7 @@
     <col min="6" max="6" width="13.96875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="20.828125" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="15.8203125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="52.29296875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="50.4375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="12.28125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="10.59375" customWidth="true" bestFit="true"/>
@@ -696,7 +801,7 @@
         <v>46</v>
       </c>
       <c r="E2" t="n" s="2">
-        <v>28430.030026724537</v>
+        <v>28430.16734834491</v>
       </c>
       <c r="F2" t="s">
         <v>47</v>
@@ -734,7 +839,7 @@
         <v>56</v>
       </c>
       <c r="E3" t="n" s="2">
-        <v>28430.030026724537</v>
+        <v>28430.16734834491</v>
       </c>
       <c r="F3" t="s">
         <v>57</v>
@@ -772,7 +877,7 @@
         <v>46</v>
       </c>
       <c r="E4" t="n" s="2">
-        <v>28430.030026724537</v>
+        <v>28430.16734834491</v>
       </c>
       <c r="F4" t="s">
         <v>66</v>
@@ -810,7 +915,7 @@
         <v>56</v>
       </c>
       <c r="E5" t="n" s="2">
-        <v>28430.030026724537</v>
+        <v>28430.16734834491</v>
       </c>
       <c r="F5" t="s">
         <v>74</v>
@@ -848,7 +953,7 @@
         <v>56</v>
       </c>
       <c r="E6" t="n" s="2">
-        <v>28430.030026724537</v>
+        <v>28430.16734834491</v>
       </c>
       <c r="F6" t="s">
         <v>83</v>
@@ -886,7 +991,7 @@
         <v>56</v>
       </c>
       <c r="E7" t="n" s="2">
-        <v>28430.030026724537</v>
+        <v>28430.16734834491</v>
       </c>
       <c r="F7" t="s">
         <v>90</v>
@@ -924,7 +1029,7 @@
         <v>56</v>
       </c>
       <c r="E8" t="n" s="2">
-        <v>28430.030026724537</v>
+        <v>28430.16734834491</v>
       </c>
       <c r="F8" t="s">
         <v>90</v>
@@ -970,7 +1075,7 @@
     <col min="7" max="7" width="5.77734375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="21.96875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="15.25" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="50.48046875" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="52.00390625" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="20.04296875" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="18.6328125" customWidth="true" bestFit="true"/>
@@ -1034,8 +1139,8 @@
       <c r="D2" t="s">
         <v>46</v>
       </c>
-      <c r="E2" t="n" s="2">
-        <v>28430.030026724537</v>
+      <c r="E2" t="n" s="3">
+        <v>28430.16734834491</v>
       </c>
       <c r="F2" t="s">
         <v>103</v>
@@ -1078,8 +1183,8 @@
       <c r="D3" t="s">
         <v>46</v>
       </c>
-      <c r="E3" t="n" s="2">
-        <v>28430.030026724537</v>
+      <c r="E3" t="n" s="3">
+        <v>28430.16734834491</v>
       </c>
       <c r="F3" t="s">
         <v>112</v>
@@ -1122,8 +1227,8 @@
       <c r="D4" t="s">
         <v>56</v>
       </c>
-      <c r="E4" t="n" s="2">
-        <v>28430.030026724537</v>
+      <c r="E4" t="n" s="3">
+        <v>28430.16734834491</v>
       </c>
       <c r="F4" t="s">
         <v>121</v>
@@ -1166,8 +1271,8 @@
       <c r="D5" t="s">
         <v>56</v>
       </c>
-      <c r="E5" t="n" s="2">
-        <v>28430.030026724537</v>
+      <c r="E5" t="n" s="3">
+        <v>28430.16734834491</v>
       </c>
       <c r="F5" t="s">
         <v>129</v>
@@ -1210,8 +1315,8 @@
       <c r="D6" t="s">
         <v>46</v>
       </c>
-      <c r="E6" t="n" s="2">
-        <v>28430.030026724537</v>
+      <c r="E6" t="n" s="3">
+        <v>28430.16734834491</v>
       </c>
       <c r="F6" t="s">
         <v>137</v>
@@ -1262,7 +1367,7 @@
     <col min="6" max="6" width="13.96875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="23.7265625" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="14.23828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="51.61328125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="53.62890625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="18.09375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="17.89453125" customWidth="true" bestFit="true"/>
@@ -1323,8 +1428,8 @@
       <c r="D2" t="s">
         <v>56</v>
       </c>
-      <c r="E2" t="n" s="2">
-        <v>28430.030026724537</v>
+      <c r="E2" t="n" s="4">
+        <v>28430.16734834491</v>
       </c>
       <c r="F2" t="s">
         <v>145</v>
@@ -1364,8 +1469,8 @@
       <c r="D3" t="s">
         <v>46</v>
       </c>
-      <c r="E3" t="n" s="2">
-        <v>28430.030026724537</v>
+      <c r="E3" t="n" s="4">
+        <v>28430.16734834491</v>
       </c>
       <c r="F3" t="s">
         <v>153</v>
@@ -1405,8 +1510,8 @@
       <c r="D4" t="s">
         <v>56</v>
       </c>
-      <c r="E4" t="n" s="2">
-        <v>28430.030026724537</v>
+      <c r="E4" t="n" s="4">
+        <v>28430.16734834491</v>
       </c>
       <c r="F4" t="s">
         <v>162</v>
@@ -1446,7 +1551,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="6.609375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="20.6328125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="23.8125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="25.03515625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="13.63671875" customWidth="true" bestFit="true"/>
@@ -1456,7 +1561,7 @@
     <col min="8" max="8" width="15.09375" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="7.578125" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="11.4609375" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="7.515625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="11.19921875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="12.79296875" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="15.6640625" customWidth="true" bestFit="true"/>
   </cols>
@@ -1503,114 +1608,122 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>11254.0</v>
+      <c r="A2" t="s">
+        <v>169</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
       </c>
       <c r="E2"/>
       <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>172</v>
+      </c>
+      <c r="H2" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>173</v>
+      </c>
+      <c r="J2" t="s">
+        <v>174</v>
+      </c>
+      <c r="K2" t="s">
+        <v>175</v>
+      </c>
+      <c r="L2" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D3" t="b">
         <v>0</v>
       </c>
-      <c r="G2"/>
-      <c r="H2" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="I2" t="s">
-        <v>171</v>
-      </c>
-      <c r="J2" t="n">
-        <v>250.0</v>
-      </c>
-      <c r="K2" t="n">
+      <c r="E3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H3" t="n">
         <v>7.0</v>
       </c>
-      <c r="L2" t="s">
-        <v>172</v>
-      </c>
-      <c r="M2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>11254.0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C3" t="s">
-        <v>170</v>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3"/>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3"/>
-      <c r="H3" t="n">
-        <v>4.0</v>
-      </c>
       <c r="I3" t="s">
-        <v>171</v>
-      </c>
-      <c r="J3" t="n">
-        <v>250.0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="L3" t="s">
-        <v>172</v>
-      </c>
-      <c r="M3" t="s">
-        <v>173</v>
+        <v>180</v>
+      </c>
+      <c r="J3" t="s">
+        <v>181</v>
+      </c>
+      <c r="K3" t="s">
+        <v>182</v>
+      </c>
+      <c r="L3" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>5.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>11254.0</v>
+      <c r="A4" t="s">
+        <v>183</v>
       </c>
       <c r="B4" t="s">
-        <v>169</v>
+        <v>184</v>
       </c>
       <c r="C4" t="s">
-        <v>170</v>
+        <v>185</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
       </c>
       <c r="E4"/>
       <c r="F4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4"/>
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>186</v>
+      </c>
       <c r="H4" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="I4" t="s">
-        <v>171</v>
-      </c>
-      <c r="J4" t="n">
-        <v>250.0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="L4" t="s">
-        <v>172</v>
-      </c>
-      <c r="M4" t="s">
-        <v>173</v>
+        <v>187</v>
+      </c>
+      <c r="J4" t="s">
+        <v>188</v>
+      </c>
+      <c r="K4" t="s">
+        <v>189</v>
+      </c>
+      <c r="L4" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>5.0</v>
       </c>
     </row>
   </sheetData>
@@ -1626,7 +1739,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="6.609375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="20.70703125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="23.8125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="25.03515625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="13.63671875" customWidth="true" bestFit="true"/>
@@ -1634,7 +1747,7 @@
     <col min="6" max="6" width="11.921875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="30.76171875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="15.09375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="7.578125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="6.4375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="12.79296875" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="15.6640625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="13.515625" customWidth="true" bestFit="true"/>
@@ -1683,14 +1796,14 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>11254.0</v>
+      <c r="A2" t="s">
+        <v>190</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
       <c r="C2" t="s">
-        <v>170</v>
+        <v>192</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1704,67 +1817,69 @@
         <v>2.0</v>
       </c>
       <c r="I2" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="J2" t="n">
-        <v>250.0</v>
+        <v>100.0</v>
       </c>
       <c r="K2" t="n">
-        <v>7.0</v>
+        <v>5.0</v>
       </c>
       <c r="L2" t="n">
         <v>56.5</v>
       </c>
       <c r="M2" t="n">
-        <v>15.1</v>
+        <v>36.1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>11254.0</v>
+      <c r="A3" t="s">
+        <v>193</v>
       </c>
       <c r="B3" t="s">
-        <v>174</v>
+        <v>194</v>
       </c>
       <c r="C3" t="s">
-        <v>170</v>
+        <v>195</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
       </c>
       <c r="E3"/>
       <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3"/>
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>172</v>
+      </c>
       <c r="H3" t="n">
         <v>2.0</v>
       </c>
       <c r="I3" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="J3" t="n">
-        <v>250.0</v>
+        <v>100.0</v>
       </c>
       <c r="K3" t="n">
-        <v>7.0</v>
+        <v>5.0</v>
       </c>
       <c r="L3" t="n">
-        <v>56.5</v>
+        <v>65.0</v>
       </c>
       <c r="M3" t="n">
-        <v>15.1</v>
+        <v>32.24</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>11254.0</v>
+      <c r="A4" t="s">
+        <v>196</v>
       </c>
       <c r="B4" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
       <c r="C4" t="s">
-        <v>170</v>
+        <v>198</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -1778,19 +1893,19 @@
         <v>2.0</v>
       </c>
       <c r="I4" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="J4" t="n">
-        <v>250.0</v>
+        <v>100.0</v>
       </c>
       <c r="K4" t="n">
-        <v>7.0</v>
+        <v>5.0</v>
       </c>
       <c r="L4" t="n">
-        <v>56.5</v>
+        <v>70.5</v>
       </c>
       <c r="M4" t="n">
-        <v>15.1</v>
+        <v>25.1</v>
       </c>
     </row>
   </sheetData>
@@ -1806,7 +1921,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="6.609375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="20.3984375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="23.8125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="25.03515625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="13.63671875" customWidth="true" bestFit="true"/>
@@ -1814,10 +1929,10 @@
     <col min="6" max="6" width="11.921875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="30.76171875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="15.09375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="7.578125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="6.44921875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="12.79296875" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="15.6640625" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="11.7890625" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="13.69921875" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="15.57421875" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="17.53515625" customWidth="true" bestFit="true"/>
   </cols>
@@ -1867,37 +1982,41 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>11254.0</v>
+      <c r="A2" t="s">
+        <v>199</v>
       </c>
       <c r="B2" t="s">
-        <v>176</v>
+        <v>200</v>
       </c>
       <c r="C2" t="s">
-        <v>170</v>
+        <v>201</v>
       </c>
       <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>202</v>
+      </c>
+      <c r="F2" t="b">
         <v>1</v>
       </c>
-      <c r="E2"/>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2"/>
+      <c r="G2" t="s">
+        <v>172</v>
+      </c>
       <c r="H2" t="n">
-        <v>7.0</v>
+        <v>30.0</v>
       </c>
       <c r="I2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="J2" t="n">
-        <v>250.0</v>
+        <v>100.0</v>
       </c>
       <c r="K2" t="n">
-        <v>7.0</v>
+        <v>5.0</v>
       </c>
       <c r="L2" t="s">
-        <v>177</v>
+        <v>200</v>
       </c>
       <c r="M2" t="b">
         <v>1</v>
@@ -1907,54 +2026,58 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>11254.0</v>
+      <c r="A3" t="s">
+        <v>203</v>
       </c>
       <c r="B3" t="s">
-        <v>176</v>
+        <v>204</v>
       </c>
       <c r="C3" t="s">
-        <v>170</v>
+        <v>205</v>
       </c>
       <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F3" t="b">
         <v>1</v>
       </c>
-      <c r="E3"/>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3"/>
+      <c r="G3" t="s">
+        <v>206</v>
+      </c>
       <c r="H3" t="n">
-        <v>7.0</v>
+        <v>70.0</v>
       </c>
       <c r="I3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="J3" t="n">
-        <v>250.0</v>
+        <v>100.0</v>
       </c>
       <c r="K3" t="n">
-        <v>7.0</v>
+        <v>5.0</v>
       </c>
       <c r="L3" t="s">
-        <v>177</v>
+        <v>207</v>
       </c>
       <c r="M3" t="b">
         <v>1</v>
       </c>
       <c r="N3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>11254.0</v>
+      <c r="A4" t="s">
+        <v>208</v>
       </c>
       <c r="B4" t="s">
-        <v>176</v>
+        <v>209</v>
       </c>
       <c r="C4" t="s">
-        <v>170</v>
+        <v>210</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -1965,19 +2088,19 @@
       </c>
       <c r="G4"/>
       <c r="H4" t="n">
-        <v>7.0</v>
+        <v>40.0</v>
       </c>
       <c r="I4" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="J4" t="n">
-        <v>250.0</v>
+        <v>100.0</v>
       </c>
       <c r="K4" t="n">
-        <v>7.0</v>
+        <v>5.0</v>
       </c>
       <c r="L4" t="s">
-        <v>177</v>
+        <v>211</v>
       </c>
       <c r="M4" t="b">
         <v>1</v>
@@ -2002,7 +2125,7 @@
     <col min="1" max="1" width="19.23828125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="17.96484375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="15.9375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="9.8671875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="19.21484375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="16.125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="20.58984375" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="11.5390625" customWidth="true" bestFit="true"/>
@@ -2033,19 +2156,19 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>178</v>
+        <v>212</v>
       </c>
       <c r="B2" t="s">
-        <v>179</v>
+        <v>213</v>
       </c>
       <c r="C2" t="n">
         <v>10.0</v>
       </c>
       <c r="D2" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="E2" t="s">
-        <v>181</v>
+        <v>214</v>
       </c>
       <c r="F2" t="n">
         <v>15.25</v>
@@ -2056,42 +2179,42 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>178</v>
+        <v>212</v>
       </c>
       <c r="B3" t="s">
-        <v>179</v>
+        <v>215</v>
       </c>
       <c r="C3" t="n">
-        <v>10.0</v>
+        <v>36.0</v>
       </c>
       <c r="D3" t="s">
-        <v>180</v>
+        <v>216</v>
       </c>
       <c r="E3" t="s">
-        <v>181</v>
+        <v>214</v>
       </c>
       <c r="F3" t="n">
         <v>15.25</v>
       </c>
       <c r="G3" t="n">
-        <v>515.25</v>
+        <v>1815.25</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>178</v>
+        <v>212</v>
       </c>
       <c r="B4" t="s">
-        <v>179</v>
+        <v>213</v>
       </c>
       <c r="C4" t="n">
         <v>10.0</v>
       </c>
       <c r="D4" t="s">
-        <v>180</v>
+        <v>216</v>
       </c>
       <c r="E4" t="s">
-        <v>181</v>
+        <v>214</v>
       </c>
       <c r="F4" t="n">
         <v>15.25</v>

</xml_diff>

<commit_message>
[Anmol Singh]Class ExcelWriter-Data Duplication error Resolved(static keyword is the root cause)
</commit_message>
<xml_diff>
--- a/Car_Rental_System.xlsx
+++ b/Car_Rental_System.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="216">
   <si>
     <t>ID</t>
   </si>
@@ -170,7 +170,7 @@
     <t>Me_AnmolSingh</t>
   </si>
   <si>
-    <t>MLsex7I0KUyCAevDbMImc1XBcC+gVvs+jIdPx6nuGCA=</t>
+    <t>8ORupWyAWxOCwZ92mHnxlLl9RhVeZy6hMd3k26bnxQA=</t>
   </si>
   <si>
     <t>ghtutgd</t>
@@ -200,7 +200,7 @@
     <t>Me_AmanKaur</t>
   </si>
   <si>
-    <t>uFomyJUvMUbjAE6BpcEixEy0H9/RDJ2ogHuy+awlF1E=</t>
+    <t>A0gFS9YPIidGmiwG3rI9Ipo2YAFVvvfcis7XPa+pA4A=</t>
   </si>
   <si>
     <t>458954hgtfr</t>
@@ -227,7 +227,7 @@
     <t>Me_inshant</t>
   </si>
   <si>
-    <t>tmKaj15OEV7SG2etsSgEDozGWQqT5JWURm9jLr3lrAY=</t>
+    <t>chSF5+/lJt6W6ZyvIDn9Q1FP1fHsy7B3LAEDpx0FIEw=</t>
   </si>
   <si>
     <t>inshant</t>
@@ -251,7 +251,7 @@
     <t>Me_Monica</t>
   </si>
   <si>
-    <t>D1kcEXZRDAH7f7rwj/wan5EPsn2zjKD/4U9hc+i4glU=</t>
+    <t>vK0RIBs47cxmRuL82g99fgogF/91BiHhxrRzEyIoRc8=</t>
   </si>
   <si>
     <t>5485lkjhy</t>
@@ -278,7 +278,7 @@
     <t>Ikroop_Virk</t>
   </si>
   <si>
-    <t>Oxh7ejzPqvg/rgaXMoCXwZnTiZxcJjJ/eOaHGLwSFdo=</t>
+    <t>0HIks10ObiMPLrKy5WQPsJZAggWjHpzIj8IN3TctahM=</t>
   </si>
   <si>
     <t>virkikroop</t>
@@ -299,7 +299,7 @@
     <t>Me_kritima</t>
   </si>
   <si>
-    <t>AUii3G7lRdxcqfxDmAXWgKY7jIrSe0ba4GpuKd+2cDo=</t>
+    <t>gXUp/hqhsg7YQkX8uH3H9trj/I0JE0CUwSDcFxXvUVQ=</t>
   </si>
   <si>
     <t>5475lkmnj</t>
@@ -314,7 +314,7 @@
     <t>Me_param</t>
   </si>
   <si>
-    <t>5f9LzyL1RiEP29LxAIWL51+UCHD9rSVfN8foLcaqBNw=</t>
+    <t>fmvzmvVxlYOSGFuF8TEim7iIZQ1RAnexcyVRCP+tI+4=</t>
   </si>
   <si>
     <t>paramkaur</t>
@@ -338,7 +338,7 @@
     <t>KumarShanu</t>
   </si>
   <si>
-    <t>YM46aLrktAM0L2Ijzatm+bPD7ekLyMUBbyFLr7yS7IA=</t>
+    <t>qTvB1tdNSihRNnQciOXHtpVTR805OKBLnDQuIOH4gKw=</t>
   </si>
   <si>
     <t>kjhujh</t>
@@ -365,7 +365,7 @@
     <t>Jordan_Micheal</t>
   </si>
   <si>
-    <t>4+P61+ueT1J/pZBdZ4CIX+f59mAUqWm94DLbAh+NhJM=</t>
+    <t>pz02rBQF3CBtLxbMiKKG4q0/prqxsusNPpB3qeKlwyg=</t>
   </si>
   <si>
     <t>dfgtre3</t>
@@ -392,7 +392,7 @@
     <t>michelle</t>
   </si>
   <si>
-    <t>QJjyPUmHZ1HyOujHmG/VTzBJg2JLKKn7yaJgo3Ci9x8=</t>
+    <t>Sh+4x4/BZ/XEgbJUmJSGev+qhyrUbW9KftowcxL1YlY=</t>
   </si>
   <si>
     <t>1254gytr</t>
@@ -416,7 +416,7 @@
     <t>SherinG</t>
   </si>
   <si>
-    <t>jUatMlThD/JbO/2I7Zhc12pqnzP7ni2NSNLZP0yRT0s=</t>
+    <t>jqRS0opZAo2C/2VOjMFc/XeiC4wT8qba+ETLJ7tP+Ac=</t>
   </si>
   <si>
     <t>524plo;</t>
@@ -440,7 +440,7 @@
     <t>JainSaab</t>
   </si>
   <si>
-    <t>jZCWcGTlimZFMZBGAI2sSzvneg716kEjXn59Fc8Qn/4=</t>
+    <t>kFAYkSvsL508eUkwLIW2yAM6pWB8+hC5jNpG0jACxPw=</t>
   </si>
   <si>
     <t>ppo;;lko</t>
@@ -458,7 +458,7 @@
     <t>6723367567</t>
   </si>
   <si>
-    <t>tk1VQQSYIAyUHCJ729eunNq71X9Id7pEPbwsROPUJ6I=</t>
+    <t>ndHUnHZuQGjeGvx9O17ci6OHclvNeO1aC51UIRwmWgk=</t>
   </si>
   <si>
     <t>ghat</t>
@@ -485,7 +485,7 @@
     <t>gillingum@gillingum.com</t>
   </si>
   <si>
-    <t>VKxJ0X+3sFilno3aIXMHvj1MngEsKDMQF5v6XAjGXB4=</t>
+    <t>FPCScMKVq8Bq+FPrF0pynR6WeFGepKcIucJ/WAwK4ZE=</t>
   </si>
   <si>
     <t>dhobi_ghat</t>
@@ -512,7 +512,7 @@
     <t>careem@me.com</t>
   </si>
   <si>
-    <t>Z79RO7SfLmurq8+Qmv3MiFgD1gbPQWLQkM2E8m1p0gg=</t>
+    <t>cjebWLk/782JjOf5MVfIBFANzBhcZlN7x8xcSXhHxyY=</t>
   </si>
   <si>
     <t>Gaziattack</t>
@@ -557,7 +557,7 @@
     <t>Mercedes</t>
   </si>
   <si>
-    <t>IP5</t>
+    <t>Micheal</t>
   </si>
   <si>
     <t>Petrol</t>
@@ -578,7 +578,7 @@
     <t>Hyundai</t>
   </si>
   <si>
-    <t>IP4</t>
+    <t>Ramesh</t>
   </si>
   <si>
     <t>Electric</t>
@@ -608,6 +608,9 @@
     <t>BMW</t>
   </si>
   <si>
+    <t>IP2</t>
+  </si>
+  <si>
     <t>1J4BA6H11AL289387</t>
   </si>
   <si>
@@ -626,9 +629,6 @@
     <t>BusCompany-A</t>
   </si>
   <si>
-    <t>Micheal</t>
-  </si>
-  <si>
     <t>1G1ZT548X5F147693</t>
   </si>
   <si>
@@ -636,9 +636,6 @@
   </si>
   <si>
     <t>BusCompany-B</t>
-  </si>
-  <si>
-    <t>IP3</t>
   </si>
   <si>
     <t>DoubleDecker</t>
@@ -743,7 +740,7 @@
     <col min="6" max="6" width="13.96875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="20.828125" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="15.8203125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="50.4375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="53.484375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="12.28125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="10.59375" customWidth="true" bestFit="true"/>
@@ -801,7 +798,7 @@
         <v>46</v>
       </c>
       <c r="E2" t="n" s="2">
-        <v>28430.16734834491</v>
+        <v>35749.17427505787</v>
       </c>
       <c r="F2" t="s">
         <v>47</v>
@@ -839,7 +836,7 @@
         <v>56</v>
       </c>
       <c r="E3" t="n" s="2">
-        <v>28430.16734834491</v>
+        <v>35637.17427505787</v>
       </c>
       <c r="F3" t="s">
         <v>57</v>
@@ -877,7 +874,7 @@
         <v>46</v>
       </c>
       <c r="E4" t="n" s="2">
-        <v>28430.16734834491</v>
+        <v>35445.17427505787</v>
       </c>
       <c r="F4" t="s">
         <v>66</v>
@@ -915,7 +912,7 @@
         <v>56</v>
       </c>
       <c r="E5" t="n" s="2">
-        <v>28430.16734834491</v>
+        <v>35602.17427505787</v>
       </c>
       <c r="F5" t="s">
         <v>74</v>
@@ -953,7 +950,7 @@
         <v>56</v>
       </c>
       <c r="E6" t="n" s="2">
-        <v>28430.16734834491</v>
+        <v>34912.17427505787</v>
       </c>
       <c r="F6" t="s">
         <v>83</v>
@@ -991,7 +988,7 @@
         <v>56</v>
       </c>
       <c r="E7" t="n" s="2">
-        <v>28430.16734834491</v>
+        <v>35567.17427505787</v>
       </c>
       <c r="F7" t="s">
         <v>90</v>
@@ -1029,7 +1026,7 @@
         <v>56</v>
       </c>
       <c r="E8" t="n" s="2">
-        <v>28430.16734834491</v>
+        <v>33783.17427505787</v>
       </c>
       <c r="F8" t="s">
         <v>90</v>
@@ -1075,7 +1072,7 @@
     <col min="7" max="7" width="5.77734375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="21.96875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="15.25" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="52.00390625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="51.72265625" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="20.04296875" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="18.6328125" customWidth="true" bestFit="true"/>
@@ -1140,7 +1137,7 @@
         <v>46</v>
       </c>
       <c r="E2" t="n" s="3">
-        <v>28430.16734834491</v>
+        <v>35735.17427505787</v>
       </c>
       <c r="F2" t="s">
         <v>103</v>
@@ -1184,7 +1181,7 @@
         <v>46</v>
       </c>
       <c r="E3" t="n" s="3">
-        <v>28430.16734834491</v>
+        <v>28476.17427505787</v>
       </c>
       <c r="F3" t="s">
         <v>112</v>
@@ -1228,7 +1225,7 @@
         <v>56</v>
       </c>
       <c r="E4" t="n" s="3">
-        <v>28430.16734834491</v>
+        <v>36936.17427505787</v>
       </c>
       <c r="F4" t="s">
         <v>121</v>
@@ -1272,7 +1269,7 @@
         <v>56</v>
       </c>
       <c r="E5" t="n" s="3">
-        <v>28430.16734834491</v>
+        <v>31279.17427505787</v>
       </c>
       <c r="F5" t="s">
         <v>129</v>
@@ -1316,7 +1313,7 @@
         <v>46</v>
       </c>
       <c r="E6" t="n" s="3">
-        <v>28430.16734834491</v>
+        <v>23923.17427505787</v>
       </c>
       <c r="F6" t="s">
         <v>137</v>
@@ -1367,7 +1364,7 @@
     <col min="6" max="6" width="13.96875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="23.7265625" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="14.23828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="53.62890625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="52.39453125" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="18.09375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="17.89453125" customWidth="true" bestFit="true"/>
@@ -1429,7 +1426,7 @@
         <v>56</v>
       </c>
       <c r="E2" t="n" s="4">
-        <v>28430.16734834491</v>
+        <v>29842.17427505787</v>
       </c>
       <c r="F2" t="s">
         <v>145</v>
@@ -1470,7 +1467,7 @@
         <v>46</v>
       </c>
       <c r="E3" t="n" s="4">
-        <v>28430.16734834491</v>
+        <v>28251.17427505787</v>
       </c>
       <c r="F3" t="s">
         <v>153</v>
@@ -1511,7 +1508,7 @@
         <v>56</v>
       </c>
       <c r="E4" t="n" s="4">
-        <v>28430.16734834491</v>
+        <v>29677.17427505787</v>
       </c>
       <c r="F4" t="s">
         <v>162</v>
@@ -1660,13 +1657,13 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>127</v>
+        <v>179</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>179</v>
+        <v>119</v>
       </c>
       <c r="H3" t="n">
         <v>7.0</v>
@@ -1820,10 +1817,10 @@
         <v>180</v>
       </c>
       <c r="J2" t="n">
-        <v>100.0</v>
+        <v>50.0</v>
       </c>
       <c r="K2" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="L2" t="n">
         <v>56.5</v>
@@ -1850,7 +1847,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>172</v>
+        <v>196</v>
       </c>
       <c r="H3" t="n">
         <v>2.0</v>
@@ -1859,10 +1856,10 @@
         <v>180</v>
       </c>
       <c r="J3" t="n">
-        <v>100.0</v>
+        <v>50.0</v>
       </c>
       <c r="K3" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="L3" t="n">
         <v>65.0</v>
@@ -1873,13 +1870,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B4" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -1896,10 +1893,10 @@
         <v>180</v>
       </c>
       <c r="J4" t="n">
-        <v>100.0</v>
+        <v>50.0</v>
       </c>
       <c r="K4" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="L4" t="n">
         <v>70.5</v>
@@ -1983,25 +1980,25 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>202</v>
+        <v>127</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>172</v>
+        <v>135</v>
       </c>
       <c r="H2" t="n">
         <v>30.0</v>
@@ -2010,13 +2007,13 @@
         <v>173</v>
       </c>
       <c r="J2" t="n">
-        <v>100.0</v>
+        <v>250.0</v>
       </c>
       <c r="K2" t="n">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="L2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="M2" t="b">
         <v>1</v>
@@ -2045,7 +2042,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>206</v>
+        <v>172</v>
       </c>
       <c r="H3" t="n">
         <v>70.0</v>
@@ -2054,13 +2051,13 @@
         <v>173</v>
       </c>
       <c r="J3" t="n">
-        <v>100.0</v>
+        <v>250.0</v>
       </c>
       <c r="K3" t="n">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="L3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M3" t="b">
         <v>1</v>
@@ -2071,13 +2068,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B4" t="s">
         <v>208</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>209</v>
-      </c>
-      <c r="C4" t="s">
-        <v>210</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -2094,13 +2091,13 @@
         <v>180</v>
       </c>
       <c r="J4" t="n">
-        <v>100.0</v>
+        <v>250.0</v>
       </c>
       <c r="K4" t="n">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="L4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="M4" t="b">
         <v>1</v>
@@ -2156,10 +2153,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" t="s">
         <v>212</v>
-      </c>
-      <c r="B2" t="s">
-        <v>213</v>
       </c>
       <c r="C2" t="n">
         <v>10.0</v>
@@ -2168,7 +2165,7 @@
         <v>171</v>
       </c>
       <c r="E2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F2" t="n">
         <v>15.25</v>
@@ -2179,19 +2176,19 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C3" t="n">
         <v>36.0</v>
       </c>
       <c r="D3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F3" t="n">
         <v>15.25</v>
@@ -2202,19 +2199,19 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B4" t="s">
         <v>212</v>
-      </c>
-      <c r="B4" t="s">
-        <v>213</v>
       </c>
       <c r="C4" t="n">
         <v>10.0</v>
       </c>
       <c r="D4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F4" t="n">
         <v>15.25</v>

</xml_diff>

<commit_message>
[Anmol Singh]Class ExcelWriter-Data Entries Done
</commit_message>
<xml_diff>
--- a/Car_Rental_System.xlsx
+++ b/Car_Rental_System.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="218">
   <si>
     <t>ID</t>
   </si>
@@ -170,7 +170,7 @@
     <t>Me_AnmolSingh</t>
   </si>
   <si>
-    <t>8ORupWyAWxOCwZ92mHnxlLl9RhVeZy6hMd3k26bnxQA=</t>
+    <t>3C79D+vaYj32ia53a/yIMtdB3bK7AGD+O3pHyJaFyeA=</t>
   </si>
   <si>
     <t>ghtutgd</t>
@@ -200,7 +200,7 @@
     <t>Me_AmanKaur</t>
   </si>
   <si>
-    <t>A0gFS9YPIidGmiwG3rI9Ipo2YAFVvvfcis7XPa+pA4A=</t>
+    <t>U/pgUDWyI0xC6wC/JtWysTVnANGdmPFu4K6QNcKbdjs=</t>
   </si>
   <si>
     <t>458954hgtfr</t>
@@ -227,7 +227,7 @@
     <t>Me_inshant</t>
   </si>
   <si>
-    <t>chSF5+/lJt6W6ZyvIDn9Q1FP1fHsy7B3LAEDpx0FIEw=</t>
+    <t>s5MltSJCPy6C8zKQMEUfJ/GFdOETtz/bx/Iy9P6HyhM=</t>
   </si>
   <si>
     <t>inshant</t>
@@ -251,7 +251,7 @@
     <t>Me_Monica</t>
   </si>
   <si>
-    <t>vK0RIBs47cxmRuL82g99fgogF/91BiHhxrRzEyIoRc8=</t>
+    <t>lY7XNYmQxZBWY/aXA5gIkmI1rL/ez4es7cSqzdN/gQU=</t>
   </si>
   <si>
     <t>5485lkjhy</t>
@@ -278,7 +278,7 @@
     <t>Ikroop_Virk</t>
   </si>
   <si>
-    <t>0HIks10ObiMPLrKy5WQPsJZAggWjHpzIj8IN3TctahM=</t>
+    <t>fJSWxEXCmhRDBrEZtTKguMFF3iDRqwOhWyEYnnl4r3k=</t>
   </si>
   <si>
     <t>virkikroop</t>
@@ -299,7 +299,7 @@
     <t>Me_kritima</t>
   </si>
   <si>
-    <t>gXUp/hqhsg7YQkX8uH3H9trj/I0JE0CUwSDcFxXvUVQ=</t>
+    <t>uqhxwYbxmsSBXLscxgqiVDnRllWb5k49UNxbbqxBpXM=</t>
   </si>
   <si>
     <t>5475lkmnj</t>
@@ -314,7 +314,7 @@
     <t>Me_param</t>
   </si>
   <si>
-    <t>fmvzmvVxlYOSGFuF8TEim7iIZQ1RAnexcyVRCP+tI+4=</t>
+    <t>SfXI/fh9O/rqKzeqQteBp3b0wtEN2ABVYAVVP7Zsaxs=</t>
   </si>
   <si>
     <t>paramkaur</t>
@@ -338,7 +338,7 @@
     <t>KumarShanu</t>
   </si>
   <si>
-    <t>qTvB1tdNSihRNnQciOXHtpVTR805OKBLnDQuIOH4gKw=</t>
+    <t>6/eVphejdhZqtC70L0f2pSbzPFA7rkDWv4uirgJaAAQ=</t>
   </si>
   <si>
     <t>kjhujh</t>
@@ -365,7 +365,7 @@
     <t>Jordan_Micheal</t>
   </si>
   <si>
-    <t>pz02rBQF3CBtLxbMiKKG4q0/prqxsusNPpB3qeKlwyg=</t>
+    <t>DTysW1q6923lJfLZqBCw4CYp8gvJy5iq6KxQ7QeC1Ss=</t>
   </si>
   <si>
     <t>dfgtre3</t>
@@ -392,7 +392,7 @@
     <t>michelle</t>
   </si>
   <si>
-    <t>Sh+4x4/BZ/XEgbJUmJSGev+qhyrUbW9KftowcxL1YlY=</t>
+    <t>U1q/xsFdSNIp5Va74NGUxTP4uIcK+XX19wxmVlRDi9E=</t>
   </si>
   <si>
     <t>1254gytr</t>
@@ -416,7 +416,7 @@
     <t>SherinG</t>
   </si>
   <si>
-    <t>jqRS0opZAo2C/2VOjMFc/XeiC4wT8qba+ETLJ7tP+Ac=</t>
+    <t>gWhDbx9PS8s48ulfljqKpfxvhX5HZXac0z50Fof8W2Q=</t>
   </si>
   <si>
     <t>524plo;</t>
@@ -440,7 +440,7 @@
     <t>JainSaab</t>
   </si>
   <si>
-    <t>kFAYkSvsL508eUkwLIW2yAM6pWB8+hC5jNpG0jACxPw=</t>
+    <t>225W0vJTfN3mMz2Vc5uPu6h+IHeoh32HCKN/HntYr3k=</t>
   </si>
   <si>
     <t>ppo;;lko</t>
@@ -458,7 +458,7 @@
     <t>6723367567</t>
   </si>
   <si>
-    <t>ndHUnHZuQGjeGvx9O17ci6OHclvNeO1aC51UIRwmWgk=</t>
+    <t>c1qsmgqjE3jXFLknje8tYQ4sBPKwPt1MbYVg9Drx+cs=</t>
   </si>
   <si>
     <t>ghat</t>
@@ -485,7 +485,7 @@
     <t>gillingum@gillingum.com</t>
   </si>
   <si>
-    <t>FPCScMKVq8Bq+FPrF0pynR6WeFGepKcIucJ/WAwK4ZE=</t>
+    <t>MonwB8RkzXkKp4234iIgtgomWHImv8qWBj1+XOPacXU=</t>
   </si>
   <si>
     <t>dhobi_ghat</t>
@@ -512,7 +512,7 @@
     <t>careem@me.com</t>
   </si>
   <si>
-    <t>cjebWLk/782JjOf5MVfIBFANzBhcZlN7x8xcSXhHxyY=</t>
+    <t>rX8+PXXUqvY2eIMQTiDlP9tyAjAjiGO3X/l/qhDKGrk=</t>
   </si>
   <si>
     <t>Gaziattack</t>
@@ -536,7 +536,7 @@
     <t>Ford</t>
   </si>
   <si>
-    <t>IP1</t>
+    <t>Ip1</t>
   </si>
   <si>
     <t>Diesel</t>
@@ -560,6 +560,9 @@
     <t>Micheal</t>
   </si>
   <si>
+    <t>Ip5</t>
+  </si>
+  <si>
     <t>Petrol</t>
   </si>
   <si>
@@ -578,7 +581,7 @@
     <t>Hyundai</t>
   </si>
   <si>
-    <t>Ramesh</t>
+    <t>Ip6</t>
   </si>
   <si>
     <t>Electric</t>
@@ -608,7 +611,7 @@
     <t>BMW</t>
   </si>
   <si>
-    <t>IP2</t>
+    <t>Ip2</t>
   </si>
   <si>
     <t>1J4BA6H11AL289387</t>
@@ -627,6 +630,9 @@
   </si>
   <si>
     <t>BusCompany-A</t>
+  </si>
+  <si>
+    <t>Ip7</t>
   </si>
   <si>
     <t>1G1ZT548X5F147693</t>
@@ -740,7 +746,7 @@
     <col min="6" max="6" width="13.96875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="20.828125" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="15.8203125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="53.484375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="51.87890625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="12.28125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="10.59375" customWidth="true" bestFit="true"/>
@@ -798,7 +804,7 @@
         <v>46</v>
       </c>
       <c r="E2" t="n" s="2">
-        <v>35749.17427505787</v>
+        <v>35749.18615758102</v>
       </c>
       <c r="F2" t="s">
         <v>47</v>
@@ -836,7 +842,7 @@
         <v>56</v>
       </c>
       <c r="E3" t="n" s="2">
-        <v>35637.17427505787</v>
+        <v>35637.18615758102</v>
       </c>
       <c r="F3" t="s">
         <v>57</v>
@@ -874,7 +880,7 @@
         <v>46</v>
       </c>
       <c r="E4" t="n" s="2">
-        <v>35445.17427505787</v>
+        <v>35445.18615758102</v>
       </c>
       <c r="F4" t="s">
         <v>66</v>
@@ -912,7 +918,7 @@
         <v>56</v>
       </c>
       <c r="E5" t="n" s="2">
-        <v>35602.17427505787</v>
+        <v>35602.18615758102</v>
       </c>
       <c r="F5" t="s">
         <v>74</v>
@@ -950,7 +956,7 @@
         <v>56</v>
       </c>
       <c r="E6" t="n" s="2">
-        <v>34912.17427505787</v>
+        <v>34912.18615758102</v>
       </c>
       <c r="F6" t="s">
         <v>83</v>
@@ -988,7 +994,7 @@
         <v>56</v>
       </c>
       <c r="E7" t="n" s="2">
-        <v>35567.17427505787</v>
+        <v>35567.18615758102</v>
       </c>
       <c r="F7" t="s">
         <v>90</v>
@@ -1026,7 +1032,7 @@
         <v>56</v>
       </c>
       <c r="E8" t="n" s="2">
-        <v>33783.17427505787</v>
+        <v>33783.18615758102</v>
       </c>
       <c r="F8" t="s">
         <v>90</v>
@@ -1072,7 +1078,7 @@
     <col min="7" max="7" width="5.77734375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="21.96875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="15.25" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="51.72265625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="50.9921875" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="20.04296875" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="18.6328125" customWidth="true" bestFit="true"/>
@@ -1137,13 +1143,13 @@
         <v>46</v>
       </c>
       <c r="E2" t="n" s="3">
-        <v>35735.17427505787</v>
+        <v>35735.18615758102</v>
       </c>
       <c r="F2" t="s">
         <v>103</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0</v>
+        <v>1923.0</v>
       </c>
       <c r="H2" t="s">
         <v>104</v>
@@ -1181,13 +1187,13 @@
         <v>46</v>
       </c>
       <c r="E3" t="n" s="3">
-        <v>28476.17427505787</v>
+        <v>28476.186157581018</v>
       </c>
       <c r="F3" t="s">
         <v>112</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0</v>
+        <v>1943.0</v>
       </c>
       <c r="H3" t="s">
         <v>113</v>
@@ -1225,13 +1231,13 @@
         <v>56</v>
       </c>
       <c r="E4" t="n" s="3">
-        <v>36936.17427505787</v>
+        <v>36936.18615758102</v>
       </c>
       <c r="F4" t="s">
         <v>121</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0</v>
+        <v>1919.0</v>
       </c>
       <c r="H4" t="s">
         <v>122</v>
@@ -1269,13 +1275,13 @@
         <v>56</v>
       </c>
       <c r="E5" t="n" s="3">
-        <v>31279.17427505787</v>
+        <v>31279.186157581018</v>
       </c>
       <c r="F5" t="s">
         <v>129</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0</v>
+        <v>1935.0</v>
       </c>
       <c r="H5" t="s">
         <v>130</v>
@@ -1313,13 +1319,13 @@
         <v>46</v>
       </c>
       <c r="E6" t="n" s="3">
-        <v>23923.17427505787</v>
+        <v>23923.186157581018</v>
       </c>
       <c r="F6" t="s">
         <v>137</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0</v>
+        <v>1955.0</v>
       </c>
       <c r="H6" t="s">
         <v>138</v>
@@ -1364,7 +1370,7 @@
     <col min="6" max="6" width="13.96875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="23.7265625" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="14.23828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="52.39453125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="52.03125" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="18.09375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="17.89453125" customWidth="true" bestFit="true"/>
@@ -1426,7 +1432,7 @@
         <v>56</v>
       </c>
       <c r="E2" t="n" s="4">
-        <v>29842.17427505787</v>
+        <v>29842.186157581018</v>
       </c>
       <c r="F2" t="s">
         <v>145</v>
@@ -1467,7 +1473,7 @@
         <v>46</v>
       </c>
       <c r="E3" t="n" s="4">
-        <v>28251.17427505787</v>
+        <v>28251.186157581018</v>
       </c>
       <c r="F3" t="s">
         <v>153</v>
@@ -1508,7 +1514,7 @@
         <v>56</v>
       </c>
       <c r="E4" t="n" s="4">
-        <v>29677.17427505787</v>
+        <v>29677.186157581018</v>
       </c>
       <c r="F4" t="s">
         <v>162</v>
@@ -1663,19 +1669,19 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>119</v>
+        <v>180</v>
       </c>
       <c r="H3" t="n">
         <v>7.0</v>
       </c>
       <c r="I3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="K3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="L3" t="n">
         <v>100.0</v>
@@ -1686,13 +1692,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C4" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -1702,19 +1708,19 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H4" t="n">
         <v>5.0</v>
       </c>
       <c r="I4" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="J4" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="K4" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="L4" t="n">
         <v>100.0</v>
@@ -1794,13 +1800,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1814,7 +1820,7 @@
         <v>2.0</v>
       </c>
       <c r="I2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J2" t="n">
         <v>50.0</v>
@@ -1831,13 +1837,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
@@ -1847,13 +1853,13 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H3" t="n">
         <v>2.0</v>
       </c>
       <c r="I3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J3" t="n">
         <v>50.0</v>
@@ -1870,13 +1876,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C4" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -1890,7 +1896,7 @@
         <v>2.0</v>
       </c>
       <c r="I4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J4" t="n">
         <v>50.0</v>
@@ -1922,7 +1928,7 @@
     <col min="2" max="2" width="23.8125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="25.03515625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="13.63671875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="8.51953125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="8.70703125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="11.921875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="30.76171875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="15.09375" customWidth="true" bestFit="true"/>
@@ -1980,13 +1986,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -1998,7 +2004,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>135</v>
+        <v>204</v>
       </c>
       <c r="H2" t="n">
         <v>30.0</v>
@@ -2013,7 +2019,7 @@
         <v>7.0</v>
       </c>
       <c r="L2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="M2" t="b">
         <v>1</v>
@@ -2024,19 +2030,19 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C3" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -2057,7 +2063,7 @@
         <v>7.0</v>
       </c>
       <c r="L3" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="M3" t="b">
         <v>1</v>
@@ -2068,13 +2074,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B4" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -2088,7 +2094,7 @@
         <v>40.0</v>
       </c>
       <c r="I4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J4" t="n">
         <v>250.0</v>
@@ -2097,7 +2103,7 @@
         <v>7.0</v>
       </c>
       <c r="L4" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="M4" t="b">
         <v>1</v>
@@ -2153,10 +2159,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C2" t="n">
         <v>10.0</v>
@@ -2165,7 +2171,7 @@
         <v>171</v>
       </c>
       <c r="E2" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F2" t="n">
         <v>15.25</v>
@@ -2176,19 +2182,19 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B3" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C3" t="n">
         <v>36.0</v>
       </c>
       <c r="D3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E3" t="s">
         <v>215</v>
-      </c>
-      <c r="E3" t="s">
-        <v>213</v>
       </c>
       <c r="F3" t="n">
         <v>15.25</v>
@@ -2199,19 +2205,19 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B4" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C4" t="n">
         <v>10.0</v>
       </c>
       <c r="D4" t="s">
+        <v>217</v>
+      </c>
+      <c r="E4" t="s">
         <v>215</v>
-      </c>
-      <c r="E4" t="s">
-        <v>213</v>
       </c>
       <c r="F4" t="n">
         <v>15.25</v>

</xml_diff>

<commit_message>
[Anmol Singh]Class ExcelWriter-Vehicle List Added to owner class
</commit_message>
<xml_diff>
--- a/Car_Rental_System.xlsx
+++ b/Car_Rental_System.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="229">
   <si>
     <t>ID</t>
   </si>
@@ -77,6 +77,9 @@
     <t>Website</t>
   </si>
   <si>
+    <t>Vehicle List</t>
+  </si>
+  <si>
     <t>VIN</t>
   </si>
   <si>
@@ -170,7 +173,7 @@
     <t>Me_AnmolSingh</t>
   </si>
   <si>
-    <t>3C79D+vaYj32ia53a/yIMtdB3bK7AGD+O3pHyJaFyeA=</t>
+    <t>t6cWsXANHTlLySvZiap+Hf1tSLQcch3TylG0FNaz3Q8=</t>
   </si>
   <si>
     <t>ghtutgd</t>
@@ -200,7 +203,7 @@
     <t>Me_AmanKaur</t>
   </si>
   <si>
-    <t>U/pgUDWyI0xC6wC/JtWysTVnANGdmPFu4K6QNcKbdjs=</t>
+    <t>HLR4ssAfwPI+vuwTiD0i64bbRuODVcJkp7yznFG/FLI=</t>
   </si>
   <si>
     <t>458954hgtfr</t>
@@ -227,7 +230,7 @@
     <t>Me_inshant</t>
   </si>
   <si>
-    <t>s5MltSJCPy6C8zKQMEUfJ/GFdOETtz/bx/Iy9P6HyhM=</t>
+    <t>P21meATFwsDLBo0Te+GgPcWJplvpUYbWWlmi3AntTjE=</t>
   </si>
   <si>
     <t>inshant</t>
@@ -251,7 +254,7 @@
     <t>Me_Monica</t>
   </si>
   <si>
-    <t>lY7XNYmQxZBWY/aXA5gIkmI1rL/ez4es7cSqzdN/gQU=</t>
+    <t>BJTlDUWkt/6e6HaRbh2Dfzp363LVYKOTayc/N7bpA58=</t>
   </si>
   <si>
     <t>5485lkjhy</t>
@@ -278,7 +281,7 @@
     <t>Ikroop_Virk</t>
   </si>
   <si>
-    <t>fJSWxEXCmhRDBrEZtTKguMFF3iDRqwOhWyEYnnl4r3k=</t>
+    <t>bXqSS/W8sZaZZCNL29MVBZxxpT8sQcLB0HQMXh866RE=</t>
   </si>
   <si>
     <t>virkikroop</t>
@@ -299,7 +302,7 @@
     <t>Me_kritima</t>
   </si>
   <si>
-    <t>uqhxwYbxmsSBXLscxgqiVDnRllWb5k49UNxbbqxBpXM=</t>
+    <t>oryHOLmPBl1faV0ERuRvG1DhpKol8bU4YBzaD0BAmZE=</t>
   </si>
   <si>
     <t>5475lkmnj</t>
@@ -314,7 +317,7 @@
     <t>Me_param</t>
   </si>
   <si>
-    <t>SfXI/fh9O/rqKzeqQteBp3b0wtEN2ABVYAVVP7Zsaxs=</t>
+    <t>CCIg+ylQ/HysxZ8VipuT9aBBzch5aRNjXVyfKHbxKCE=</t>
   </si>
   <si>
     <t>paramkaur</t>
@@ -338,7 +341,7 @@
     <t>KumarShanu</t>
   </si>
   <si>
-    <t>6/eVphejdhZqtC70L0f2pSbzPFA7rkDWv4uirgJaAAQ=</t>
+    <t>LT4Y4JBGH0aBPnbQkFrheN4fdtEmnAN8z9kzlPoKb8I=</t>
   </si>
   <si>
     <t>kjhujh</t>
@@ -365,7 +368,7 @@
     <t>Jordan_Micheal</t>
   </si>
   <si>
-    <t>DTysW1q6923lJfLZqBCw4CYp8gvJy5iq6KxQ7QeC1Ss=</t>
+    <t>b1JUNY13olWpEIGnQT3VsVuuDKNZ2w26+c8+ehi6dhQ=</t>
   </si>
   <si>
     <t>dfgtre3</t>
@@ -392,7 +395,7 @@
     <t>michelle</t>
   </si>
   <si>
-    <t>U1q/xsFdSNIp5Va74NGUxTP4uIcK+XX19wxmVlRDi9E=</t>
+    <t>7IkcwZH4wOYo4VDVlA7D/jxrZOzTrbq2N06YJ+IzOcA=</t>
   </si>
   <si>
     <t>1254gytr</t>
@@ -416,7 +419,7 @@
     <t>SherinG</t>
   </si>
   <si>
-    <t>gWhDbx9PS8s48ulfljqKpfxvhX5HZXac0z50Fof8W2Q=</t>
+    <t>R5b6HMwVyRcM7vagXJS0mFaksUdxu7Wl5kuBUCdZ/ns=</t>
   </si>
   <si>
     <t>524plo;</t>
@@ -440,7 +443,7 @@
     <t>JainSaab</t>
   </si>
   <si>
-    <t>225W0vJTfN3mMz2Vc5uPu6h+IHeoh32HCKN/HntYr3k=</t>
+    <t>mFcZZhU8ABk14eT/id3pTSFNB/MVJx43hYyNYwMmMns=</t>
   </si>
   <si>
     <t>ppo;;lko</t>
@@ -458,7 +461,7 @@
     <t>6723367567</t>
   </si>
   <si>
-    <t>c1qsmgqjE3jXFLknje8tYQ4sBPKwPt1MbYVg9Drx+cs=</t>
+    <t>xtQj3LNueY7B9pWTTDqsi7FWxM8IOrTnRlrHpmpV0qM=</t>
   </si>
   <si>
     <t>ghat</t>
@@ -473,6 +476,12 @@
     <t>auda.org.au</t>
   </si>
   <si>
+    <t>BMW BMX</t>
+  </si>
+  <si>
+    <t>Mercedes GWagon</t>
+  </si>
+  <si>
     <t>Gillingum</t>
   </si>
   <si>
@@ -485,7 +494,7 @@
     <t>gillingum@gillingum.com</t>
   </si>
   <si>
-    <t>MonwB8RkzXkKp4234iIgtgomWHImv8qWBj1+XOPacXU=</t>
+    <t>nqthecUEOIW2q7NYE9RfL/hiYqPuJq6++O3laGwg9oY=</t>
   </si>
   <si>
     <t>dhobi_ghat</t>
@@ -500,6 +509,21 @@
     <t>officials.org.au</t>
   </si>
   <si>
+    <t>Double-Decker</t>
+  </si>
+  <si>
+    <t>Volvo</t>
+  </si>
+  <si>
+    <t>Mini_Coach</t>
+  </si>
+  <si>
+    <t>Hyundai Civic</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>Careem</t>
   </si>
   <si>
@@ -512,7 +536,7 @@
     <t>careem@me.com</t>
   </si>
   <si>
-    <t>rX8+PXXUqvY2eIMQTiDlP9tyAjAjiGO3X/l/qhDKGrk=</t>
+    <t>pvZnFat+scpVPByniNylB9m9zrMSTsfaCfpUczY+xtU=</t>
   </si>
   <si>
     <t>Gaziattack</t>
@@ -527,6 +551,9 @@
     <t>ComapnyD.org.au</t>
   </si>
   <si>
+    <t>Bullet</t>
+  </si>
+  <si>
     <t>JHMZF1C67BS073397</t>
   </si>
   <si>
@@ -536,7 +563,7 @@
     <t>Ford</t>
   </si>
   <si>
-    <t>Ip1</t>
+    <t>IP1</t>
   </si>
   <si>
     <t>Diesel</t>
@@ -557,91 +584,85 @@
     <t>Mercedes</t>
   </si>
   <si>
+    <t>IP5</t>
+  </si>
+  <si>
+    <t>Petrol</t>
+  </si>
+  <si>
+    <t>SUV</t>
+  </si>
+  <si>
+    <t>Space-Grey</t>
+  </si>
+  <si>
+    <t>JTHKD5BH8D2168653</t>
+  </si>
+  <si>
+    <t>Civic</t>
+  </si>
+  <si>
+    <t>Hyundai</t>
+  </si>
+  <si>
+    <t>IP4</t>
+  </si>
+  <si>
+    <t>Electric</t>
+  </si>
+  <si>
+    <t>Sedan</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>1FTSW21RX8EC53647</t>
+  </si>
+  <si>
+    <t>Davidson</t>
+  </si>
+  <si>
+    <t>Harley</t>
+  </si>
+  <si>
+    <t>2HKRL1863YH598774</t>
+  </si>
+  <si>
+    <t>BMX</t>
+  </si>
+  <si>
+    <t>BMW</t>
+  </si>
+  <si>
+    <t>IP8</t>
+  </si>
+  <si>
+    <t>1J4BA6H11AL289387</t>
+  </si>
+  <si>
+    <t>Royal Enfield</t>
+  </si>
+  <si>
+    <t>5LMCJ1A97FUJ59251</t>
+  </si>
+  <si>
+    <t>BusCompany-A</t>
+  </si>
+  <si>
+    <t>1G1ZT548X5F147693</t>
+  </si>
+  <si>
+    <t>Double_decker</t>
+  </si>
+  <si>
+    <t>BusCompany-B</t>
+  </si>
+  <si>
     <t>Micheal</t>
   </si>
   <si>
-    <t>Ip5</t>
-  </si>
-  <si>
-    <t>Petrol</t>
-  </si>
-  <si>
-    <t>SUV</t>
-  </si>
-  <si>
-    <t>Space-Grey</t>
-  </si>
-  <si>
-    <t>JTHKD5BH8D2168653</t>
-  </si>
-  <si>
-    <t>Civic</t>
-  </si>
-  <si>
-    <t>Hyundai</t>
-  </si>
-  <si>
-    <t>Ip6</t>
-  </si>
-  <si>
-    <t>Electric</t>
-  </si>
-  <si>
-    <t>Sedan</t>
-  </si>
-  <si>
-    <t>Blue</t>
-  </si>
-  <si>
-    <t>1FTSW21RX8EC53647</t>
-  </si>
-  <si>
-    <t>Davidson</t>
-  </si>
-  <si>
-    <t>Harley</t>
-  </si>
-  <si>
-    <t>2HKRL1863YH598774</t>
-  </si>
-  <si>
-    <t>BMX</t>
-  </si>
-  <si>
-    <t>BMW</t>
-  </si>
-  <si>
-    <t>Ip2</t>
-  </si>
-  <si>
-    <t>1J4BA6H11AL289387</t>
-  </si>
-  <si>
-    <t>Bullet</t>
-  </si>
-  <si>
-    <t>Royal Enfield</t>
-  </si>
-  <si>
-    <t>5LMCJ1A97FUJ59251</t>
-  </si>
-  <si>
-    <t>Volvo</t>
-  </si>
-  <si>
-    <t>BusCompany-A</t>
-  </si>
-  <si>
-    <t>Ip7</t>
-  </si>
-  <si>
-    <t>1G1ZT548X5F147693</t>
-  </si>
-  <si>
-    <t>Double_decker</t>
-  </si>
-  <si>
-    <t>BusCompany-B</t>
+    <t>IP2</t>
   </si>
   <si>
     <t>DoubleDecker</t>
@@ -665,13 +686,25 @@
     <t>2020-01-25</t>
   </si>
   <si>
+    <t>CAR</t>
+  </si>
+  <si>
+    <t>2020-01-17</t>
+  </si>
+  <si>
+    <t>2020-02-20</t>
+  </si>
+  <si>
+    <t>BUS</t>
+  </si>
+  <si>
+    <t>2020-07-05</t>
+  </si>
+  <si>
+    <t>2020-07-17</t>
+  </si>
+  <si>
     <t>MOTORCYCLE</t>
-  </si>
-  <si>
-    <t>2020-02-20</t>
-  </si>
-  <si>
-    <t>Invalid Vehicle Entry</t>
   </si>
 </sst>
 </file>
@@ -746,7 +779,7 @@
     <col min="6" max="6" width="13.96875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="20.828125" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="15.8203125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="51.87890625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="52.0390625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="12.28125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="10.59375" customWidth="true" bestFit="true"/>
@@ -795,37 +828,37 @@
         <v>11514.0</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E2" t="n" s="2">
-        <v>35749.18615758102</v>
+        <v>35749.2675919213</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3">
@@ -833,37 +866,37 @@
         <v>11589.0</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E3" t="n" s="2">
-        <v>35637.18615758102</v>
+        <v>35637.2675919213</v>
       </c>
       <c r="F3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4">
@@ -871,37 +904,37 @@
         <v>11546.0</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E4" t="n" s="2">
-        <v>35445.18615758102</v>
+        <v>35445.2675919213</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="L4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5">
@@ -909,37 +942,37 @@
         <v>11575.0</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E5" t="n" s="2">
-        <v>35602.18615758102</v>
+        <v>35602.2675919213</v>
       </c>
       <c r="F5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6">
@@ -947,37 +980,37 @@
         <v>11563.0</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E6" t="n" s="2">
-        <v>34912.18615758102</v>
+        <v>34912.2675919213</v>
       </c>
       <c r="F6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7">
@@ -985,37 +1018,37 @@
         <v>11557.0</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E7" t="n" s="2">
-        <v>35567.18615758102</v>
+        <v>35567.2675919213</v>
       </c>
       <c r="F7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8">
@@ -1023,37 +1056,37 @@
         <v>11532.0</v>
       </c>
       <c r="B8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E8" t="n" s="2">
-        <v>33783.18615758102</v>
+        <v>33783.2675919213</v>
       </c>
       <c r="F8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1078,7 +1111,7 @@
     <col min="7" max="7" width="5.77734375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="21.96875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="15.25" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="50.9921875" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="52.6171875" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="20.04296875" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="18.6328125" customWidth="true" bestFit="true"/>
@@ -1134,43 +1167,43 @@
         <v>12265.0</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E2" t="n" s="3">
-        <v>35735.18615758102</v>
+        <v>35735.2675919213</v>
       </c>
       <c r="F2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G2" t="n">
         <v>1923.0</v>
       </c>
       <c r="H2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="J2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="L2" t="n">
         <v>456854.0</v>
       </c>
       <c r="M2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="N2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3">
@@ -1178,43 +1211,43 @@
         <v>12271.0</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E3" t="n" s="3">
-        <v>28476.186157581018</v>
+        <v>28476.267591921296</v>
       </c>
       <c r="F3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G3" t="n">
         <v>1943.0</v>
       </c>
       <c r="H3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L3" t="n">
         <v>854787.0</v>
       </c>
       <c r="M3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="N3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4">
@@ -1222,43 +1255,43 @@
         <v>12236.0</v>
       </c>
       <c r="B4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E4" t="n" s="3">
-        <v>36936.18615758102</v>
+        <v>36936.2675919213</v>
       </c>
       <c r="F4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G4" t="n">
         <v>1919.0</v>
       </c>
       <c r="H4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="K4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L4" t="n">
         <v>169754.0</v>
       </c>
       <c r="M4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="N4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5">
@@ -1266,43 +1299,43 @@
         <v>12451.0</v>
       </c>
       <c r="B5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E5" t="n" s="3">
-        <v>31279.186157581018</v>
+        <v>31279.267591921296</v>
       </c>
       <c r="F5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G5" t="n">
         <v>1935.0</v>
       </c>
       <c r="H5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="L5" t="n">
         <v>233256.0</v>
       </c>
       <c r="M5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="N5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6">
@@ -1310,43 +1343,43 @@
         <v>12781.0</v>
       </c>
       <c r="B6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E6" t="n" s="3">
-        <v>23923.186157581018</v>
+        <v>23923.267591921296</v>
       </c>
       <c r="F6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G6" t="n">
         <v>1955.0</v>
       </c>
       <c r="H6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="J6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="K6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="L6" t="n">
         <v>115897.0</v>
       </c>
       <c r="M6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="N6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1356,7 +1389,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1370,11 +1403,12 @@
     <col min="6" max="6" width="13.96875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="23.7265625" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="14.23828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="52.03125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="51.51171875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="18.09375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="17.89453125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="17.125" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="14.45703125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1417,46 +1451,55 @@
       <c r="M1" t="s" s="1">
         <v>18</v>
       </c>
+      <c r="N1" t="s" s="1">
+        <v>19</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>13981.0</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" t="n" s="4">
+        <v>29842.267591921296</v>
+      </c>
+      <c r="F2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" t="s">
         <v>144</v>
       </c>
-      <c r="D2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" t="n" s="4">
-        <v>29842.186157581018</v>
-      </c>
-      <c r="F2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" t="s">
-        <v>143</v>
-      </c>
       <c r="I2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="K2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="M2" t="s">
-        <v>150</v>
+        <v>151</v>
+      </c>
+      <c r="N2" t="s">
+        <v>152</v>
+      </c>
+      <c r="O2" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="3">
@@ -1464,40 +1507,55 @@
         <v>13657.0</v>
       </c>
       <c r="B3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C3" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E3" t="n" s="4">
-        <v>28251.186157581018</v>
+        <v>28251.267591921296</v>
       </c>
       <c r="F3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="G3" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="H3" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="I3" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="J3" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="K3" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="L3" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="M3" t="s">
-        <v>159</v>
+        <v>162</v>
+      </c>
+      <c r="N3" t="s">
+        <v>163</v>
+      </c>
+      <c r="O3" t="s">
+        <v>164</v>
+      </c>
+      <c r="P3" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>166</v>
+      </c>
+      <c r="R3" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="4">
@@ -1505,40 +1563,49 @@
         <v>13215.0</v>
       </c>
       <c r="B4" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="C4" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E4" t="n" s="4">
-        <v>29677.186157581018</v>
+        <v>29677.267591921296</v>
       </c>
       <c r="F4" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="G4" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="H4" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="I4" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="J4" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="K4" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="L4" t="s">
+        <v>175</v>
+      </c>
+      <c r="M4" t="s">
+        <v>176</v>
+      </c>
+      <c r="N4" t="s">
+        <v>152</v>
+      </c>
+      <c r="O4" t="s">
+        <v>177</v>
+      </c>
+      <c r="P4" t="s">
         <v>167</v>
-      </c>
-      <c r="M4" t="s">
-        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -1571,54 +1638,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="C2" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1628,19 +1695,19 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="H2" t="n">
         <v>2.0</v>
       </c>
       <c r="I2" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="J2" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="K2" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="L2" t="n">
         <v>100.0</v>
@@ -1651,37 +1718,37 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="B3" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="C3" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>179</v>
+        <v>128</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="H3" t="n">
         <v>7.0</v>
       </c>
       <c r="I3" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="J3" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="K3" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="L3" t="n">
         <v>100.0</v>
@@ -1692,13 +1759,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="B4" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="C4" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -1708,19 +1775,19 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="H4" t="n">
         <v>5.0</v>
       </c>
       <c r="I4" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="J4" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="K4" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="L4" t="n">
         <v>100.0</v>
@@ -1759,54 +1826,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="B2" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="C2" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1820,7 +1887,7 @@
         <v>2.0</v>
       </c>
       <c r="I2" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="J2" t="n">
         <v>50.0</v>
@@ -1837,13 +1904,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="B3" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="C3" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
@@ -1853,13 +1920,13 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="H3" t="n">
         <v>2.0</v>
       </c>
       <c r="I3" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="J3" t="n">
         <v>50.0</v>
@@ -1876,13 +1943,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="B4" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
       <c r="C4" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -1896,7 +1963,7 @@
         <v>2.0</v>
       </c>
       <c r="I4" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="J4" t="n">
         <v>50.0</v>
@@ -1928,7 +1995,7 @@
     <col min="2" max="2" width="23.8125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="25.03515625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="13.63671875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="8.70703125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="8.51953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="11.921875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="30.76171875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="15.09375" customWidth="true" bestFit="true"/>
@@ -1942,75 +2009,75 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="B2" t="s">
-        <v>202</v>
+        <v>164</v>
       </c>
       <c r="C2" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
       <c r="H2" t="n">
         <v>30.0</v>
       </c>
       <c r="I2" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="J2" t="n">
         <v>250.0</v>
@@ -2019,7 +2086,7 @@
         <v>7.0</v>
       </c>
       <c r="L2" t="s">
-        <v>202</v>
+        <v>164</v>
       </c>
       <c r="M2" t="b">
         <v>1</v>
@@ -2030,31 +2097,31 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="B3" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="C3" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>119</v>
+        <v>213</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>172</v>
+        <v>214</v>
       </c>
       <c r="H3" t="n">
         <v>70.0</v>
       </c>
       <c r="I3" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="J3" t="n">
         <v>250.0</v>
@@ -2063,7 +2130,7 @@
         <v>7.0</v>
       </c>
       <c r="L3" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="M3" t="b">
         <v>1</v>
@@ -2074,13 +2141,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="B4" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="C4" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -2094,7 +2161,7 @@
         <v>40.0</v>
       </c>
       <c r="I4" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="J4" t="n">
         <v>250.0</v>
@@ -2103,7 +2170,7 @@
         <v>7.0</v>
       </c>
       <c r="L4" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="M4" t="b">
         <v>1</v>
@@ -2128,102 +2195,102 @@
     <col min="1" max="1" width="19.23828125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="17.96484375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="15.9375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="19.21484375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="14.5703125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="16.125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="20.58984375" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="11.5390625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="12.7421875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="B2" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="C2" t="n">
         <v>10.0</v>
       </c>
       <c r="D2" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="E2" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="F2" t="n">
-        <v>15.25</v>
+        <v>55.18000030517578</v>
       </c>
       <c r="G2" t="n">
-        <v>515.25</v>
+        <v>1275.9000244140625</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="B3" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="C3" t="n">
-        <v>36.0</v>
+        <v>34.0</v>
       </c>
       <c r="D3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E3" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="F3" t="n">
         <v>15.25</v>
       </c>
       <c r="G3" t="n">
-        <v>1815.25</v>
+        <v>8606.75</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>213</v>
+        <v>226</v>
       </c>
       <c r="B4" t="s">
-        <v>214</v>
+        <v>227</v>
       </c>
       <c r="C4" t="n">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="D4" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="E4" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
       <c r="F4" t="n">
-        <v>15.25</v>
+        <v>36.7400016784668</v>
       </c>
       <c r="G4" t="n">
-        <v>515.25</v>
+        <v>636.739990234375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Anmol Singh]Class VehicleRent-Customer-vehicle relation build
</commit_message>
<xml_diff>
--- a/Car_Rental_System.xlsx
+++ b/Car_Rental_System.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="219">
   <si>
     <t>ID</t>
   </si>
@@ -134,6 +134,9 @@
     <t>Wifi Available</t>
   </si>
   <si>
+    <t>Customer</t>
+  </si>
+  <si>
     <t>Rent Start Date</t>
   </si>
   <si>
@@ -173,7 +176,7 @@
     <t>Me_AnmolSingh</t>
   </si>
   <si>
-    <t>t6cWsXANHTlLySvZiap+Hf1tSLQcch3TylG0FNaz3Q8=</t>
+    <t>DVLDDVM4L+1jj3a69z/cpAfQlLlVfuUlIkgEvd90w2g=</t>
   </si>
   <si>
     <t>ghtutgd</t>
@@ -203,7 +206,7 @@
     <t>Me_AmanKaur</t>
   </si>
   <si>
-    <t>HLR4ssAfwPI+vuwTiD0i64bbRuODVcJkp7yznFG/FLI=</t>
+    <t>6OgKVsE1y+h1P2SVJz0aInXYb1kK5wZkFUZ2eWzwtBM=</t>
   </si>
   <si>
     <t>458954hgtfr</t>
@@ -230,7 +233,7 @@
     <t>Me_inshant</t>
   </si>
   <si>
-    <t>P21meATFwsDLBo0Te+GgPcWJplvpUYbWWlmi3AntTjE=</t>
+    <t>tqTJTtko45JlgSn9GvNDI6pg7698O6w6NzLyN4b/Alg=</t>
   </si>
   <si>
     <t>inshant</t>
@@ -254,7 +257,7 @@
     <t>Me_Monica</t>
   </si>
   <si>
-    <t>BJTlDUWkt/6e6HaRbh2Dfzp363LVYKOTayc/N7bpA58=</t>
+    <t>V40edMd/eJipC7VUDTnNGIkHlumaqe/h1K/jh9MhGUg=</t>
   </si>
   <si>
     <t>5485lkjhy</t>
@@ -281,7 +284,7 @@
     <t>Ikroop_Virk</t>
   </si>
   <si>
-    <t>bXqSS/W8sZaZZCNL29MVBZxxpT8sQcLB0HQMXh866RE=</t>
+    <t>ZaZkerPOx0xD9w0rwLYgRDV+2mLieQY63rzhVpcGNGg=</t>
   </si>
   <si>
     <t>virkikroop</t>
@@ -302,7 +305,7 @@
     <t>Me_kritima</t>
   </si>
   <si>
-    <t>oryHOLmPBl1faV0ERuRvG1DhpKol8bU4YBzaD0BAmZE=</t>
+    <t>kGkL2v4KExuxL3+7BRUFyiFUo8t1p0F5xpMR9J7UxOU=</t>
   </si>
   <si>
     <t>5475lkmnj</t>
@@ -317,7 +320,7 @@
     <t>Me_param</t>
   </si>
   <si>
-    <t>CCIg+ylQ/HysxZ8VipuT9aBBzch5aRNjXVyfKHbxKCE=</t>
+    <t>LMYaZZ1FON6sEqKJO1o+P/Rly/S/emGVnqtjnfunzfk=</t>
   </si>
   <si>
     <t>paramkaur</t>
@@ -341,7 +344,7 @@
     <t>KumarShanu</t>
   </si>
   <si>
-    <t>LT4Y4JBGH0aBPnbQkFrheN4fdtEmnAN8z9kzlPoKb8I=</t>
+    <t>iPYbaG+xNFK4vT73eIlo2HpLgCaNWUS7OhK+QqhyT3Y=</t>
   </si>
   <si>
     <t>kjhujh</t>
@@ -368,7 +371,7 @@
     <t>Jordan_Micheal</t>
   </si>
   <si>
-    <t>b1JUNY13olWpEIGnQT3VsVuuDKNZ2w26+c8+ehi6dhQ=</t>
+    <t>US5lSqazra80k2WgZYUXWz/cEeH3MOYgtbQeHVhLWSM=</t>
   </si>
   <si>
     <t>dfgtre3</t>
@@ -395,7 +398,7 @@
     <t>michelle</t>
   </si>
   <si>
-    <t>7IkcwZH4wOYo4VDVlA7D/jxrZOzTrbq2N06YJ+IzOcA=</t>
+    <t>EiLI9x3onDSW0W4HLlZqfF6GiSFQs93D4ycCHrQU9/g=</t>
   </si>
   <si>
     <t>1254gytr</t>
@@ -419,7 +422,7 @@
     <t>SherinG</t>
   </si>
   <si>
-    <t>R5b6HMwVyRcM7vagXJS0mFaksUdxu7Wl5kuBUCdZ/ns=</t>
+    <t>fBNxOejy01MA8AWXJIRhrVZ7FWsBdKskfnXj+MS9n6o=</t>
   </si>
   <si>
     <t>524plo;</t>
@@ -443,7 +446,7 @@
     <t>JainSaab</t>
   </si>
   <si>
-    <t>mFcZZhU8ABk14eT/id3pTSFNB/MVJx43hYyNYwMmMns=</t>
+    <t>Th1BuydHm9kvBc0GqTwKTUPvs5vAUmXVM2HWgZuL6ac=</t>
   </si>
   <si>
     <t>ppo;;lko</t>
@@ -461,7 +464,7 @@
     <t>6723367567</t>
   </si>
   <si>
-    <t>xtQj3LNueY7B9pWTTDqsi7FWxM8IOrTnRlrHpmpV0qM=</t>
+    <t>1JVFsnlSA0Xczh9kgiCeDiU5FF50Vdvek7QX+jb2i7g=</t>
   </si>
   <si>
     <t>ghat</t>
@@ -476,12 +479,6 @@
     <t>auda.org.au</t>
   </si>
   <si>
-    <t>BMW BMX</t>
-  </si>
-  <si>
-    <t>Mercedes GWagon</t>
-  </si>
-  <si>
     <t>Gillingum</t>
   </si>
   <si>
@@ -494,7 +491,7 @@
     <t>gillingum@gillingum.com</t>
   </si>
   <si>
-    <t>nqthecUEOIW2q7NYE9RfL/hiYqPuJq6++O3laGwg9oY=</t>
+    <t>euiWnjng+cCi5xqyMB8QNkjbS4xJk0fibbRiLBnNRv4=</t>
   </si>
   <si>
     <t>dhobi_ghat</t>
@@ -509,144 +506,123 @@
     <t>officials.org.au</t>
   </si>
   <si>
-    <t>Double-Decker</t>
+    <t>Careem</t>
+  </si>
+  <si>
+    <t>Nazi</t>
+  </si>
+  <si>
+    <t>9988456321</t>
+  </si>
+  <si>
+    <t>careem@me.com</t>
+  </si>
+  <si>
+    <t>Vsd/VmktuG3iID8BDPbjwNbm5ZkYPqRBF5fzQH/2bw0=</t>
+  </si>
+  <si>
+    <t>Gaziattack</t>
+  </si>
+  <si>
+    <t>DCompany</t>
+  </si>
+  <si>
+    <t>2985421526</t>
+  </si>
+  <si>
+    <t>ComapnyD.org.au</t>
+  </si>
+  <si>
+    <t>JHMZF1C67BS073397</t>
+  </si>
+  <si>
+    <t>Mustang</t>
+  </si>
+  <si>
+    <t>Ford</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>Diesel</t>
+  </si>
+  <si>
+    <t>Sport</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>5TBRU34155S423198</t>
+  </si>
+  <si>
+    <t>G-Wagon</t>
+  </si>
+  <si>
+    <t>Mercedes</t>
+  </si>
+  <si>
+    <t>Petrol</t>
+  </si>
+  <si>
+    <t>SUV</t>
+  </si>
+  <si>
+    <t>Space-Grey</t>
+  </si>
+  <si>
+    <t>JTHKD5BH8D2168653</t>
+  </si>
+  <si>
+    <t>Civic</t>
+  </si>
+  <si>
+    <t>Hyundai</t>
+  </si>
+  <si>
+    <t>Electric</t>
+  </si>
+  <si>
+    <t>Sedan</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>1FTSW21RX8EC53647</t>
+  </si>
+  <si>
+    <t>Davidson</t>
+  </si>
+  <si>
+    <t>Harley</t>
+  </si>
+  <si>
+    <t>2HKRL1863YH598774</t>
+  </si>
+  <si>
+    <t>BMX</t>
+  </si>
+  <si>
+    <t>BMW</t>
+  </si>
+  <si>
+    <t>1J4BA6H11AL289387</t>
+  </si>
+  <si>
+    <t>Bullet</t>
+  </si>
+  <si>
+    <t>Royal Enfield</t>
+  </si>
+  <si>
+    <t>5LMCJ1A97FUJ59251</t>
   </si>
   <si>
     <t>Volvo</t>
   </si>
   <si>
-    <t>Mini_Coach</t>
-  </si>
-  <si>
-    <t>Hyundai Civic</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Careem</t>
-  </si>
-  <si>
-    <t>Nazi</t>
-  </si>
-  <si>
-    <t>9988456321</t>
-  </si>
-  <si>
-    <t>careem@me.com</t>
-  </si>
-  <si>
-    <t>pvZnFat+scpVPByniNylB9m9zrMSTsfaCfpUczY+xtU=</t>
-  </si>
-  <si>
-    <t>Gaziattack</t>
-  </si>
-  <si>
-    <t>DCompany</t>
-  </si>
-  <si>
-    <t>2985421526</t>
-  </si>
-  <si>
-    <t>ComapnyD.org.au</t>
-  </si>
-  <si>
-    <t>Bullet</t>
-  </si>
-  <si>
-    <t>JHMZF1C67BS073397</t>
-  </si>
-  <si>
-    <t>Mustang</t>
-  </si>
-  <si>
-    <t>Ford</t>
-  </si>
-  <si>
-    <t>IP1</t>
-  </si>
-  <si>
-    <t>Diesel</t>
-  </si>
-  <si>
-    <t>Sport</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>5TBRU34155S423198</t>
-  </si>
-  <si>
-    <t>G-Wagon</t>
-  </si>
-  <si>
-    <t>Mercedes</t>
-  </si>
-  <si>
-    <t>IP5</t>
-  </si>
-  <si>
-    <t>Petrol</t>
-  </si>
-  <si>
-    <t>SUV</t>
-  </si>
-  <si>
-    <t>Space-Grey</t>
-  </si>
-  <si>
-    <t>JTHKD5BH8D2168653</t>
-  </si>
-  <si>
-    <t>Civic</t>
-  </si>
-  <si>
-    <t>Hyundai</t>
-  </si>
-  <si>
-    <t>IP4</t>
-  </si>
-  <si>
-    <t>Electric</t>
-  </si>
-  <si>
-    <t>Sedan</t>
-  </si>
-  <si>
-    <t>Blue</t>
-  </si>
-  <si>
-    <t>1FTSW21RX8EC53647</t>
-  </si>
-  <si>
-    <t>Davidson</t>
-  </si>
-  <si>
-    <t>Harley</t>
-  </si>
-  <si>
-    <t>2HKRL1863YH598774</t>
-  </si>
-  <si>
-    <t>BMX</t>
-  </si>
-  <si>
-    <t>BMW</t>
-  </si>
-  <si>
-    <t>IP8</t>
-  </si>
-  <si>
-    <t>1J4BA6H11AL289387</t>
-  </si>
-  <si>
-    <t>Royal Enfield</t>
-  </si>
-  <si>
-    <t>5LMCJ1A97FUJ59251</t>
-  </si>
-  <si>
     <t>BusCompany-A</t>
   </si>
   <si>
@@ -657,12 +633,6 @@
   </si>
   <si>
     <t>BusCompany-B</t>
-  </si>
-  <si>
-    <t>Micheal</t>
-  </si>
-  <si>
-    <t>IP2</t>
   </si>
   <si>
     <t>DoubleDecker</t>
@@ -779,7 +749,7 @@
     <col min="6" max="6" width="13.96875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="20.828125" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="15.8203125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="52.0390625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="50.96875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="12.28125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="10.59375" customWidth="true" bestFit="true"/>
@@ -828,37 +798,37 @@
         <v>11514.0</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E2" t="n" s="2">
-        <v>35749.2675919213</v>
+        <v>35749.30108271991</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3">
@@ -866,37 +836,37 @@
         <v>11589.0</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E3" t="n" s="2">
-        <v>35637.2675919213</v>
+        <v>35637.30108271991</v>
       </c>
       <c r="F3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4">
@@ -904,37 +874,37 @@
         <v>11546.0</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E4" t="n" s="2">
-        <v>35445.2675919213</v>
+        <v>35445.30108271991</v>
       </c>
       <c r="F4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5">
@@ -942,37 +912,37 @@
         <v>11575.0</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E5" t="n" s="2">
-        <v>35602.2675919213</v>
+        <v>35602.30108271991</v>
       </c>
       <c r="F5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6">
@@ -980,37 +950,37 @@
         <v>11563.0</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E6" t="n" s="2">
-        <v>34912.2675919213</v>
+        <v>34912.30108271991</v>
       </c>
       <c r="F6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7">
@@ -1018,37 +988,37 @@
         <v>11557.0</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E7" t="n" s="2">
-        <v>35567.2675919213</v>
+        <v>35567.30108271991</v>
       </c>
       <c r="F7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8">
@@ -1056,37 +1026,37 @@
         <v>11532.0</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E8" t="n" s="2">
-        <v>33783.2675919213</v>
+        <v>33783.30108271991</v>
       </c>
       <c r="F8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="I8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="L8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1111,7 +1081,7 @@
     <col min="7" max="7" width="5.77734375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="21.96875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="15.25" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="52.6171875" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="53.7734375" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="20.04296875" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="18.6328125" customWidth="true" bestFit="true"/>
@@ -1167,43 +1137,43 @@
         <v>12265.0</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E2" t="n" s="3">
-        <v>35735.2675919213</v>
+        <v>35735.30108271991</v>
       </c>
       <c r="F2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G2" t="n">
         <v>1923.0</v>
       </c>
       <c r="H2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="K2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L2" t="n">
         <v>456854.0</v>
       </c>
       <c r="M2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="N2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3">
@@ -1211,43 +1181,43 @@
         <v>12271.0</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E3" t="n" s="3">
-        <v>28476.267591921296</v>
+        <v>28476.301082719907</v>
       </c>
       <c r="F3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G3" t="n">
         <v>1943.0</v>
       </c>
       <c r="H3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="K3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="L3" t="n">
         <v>854787.0</v>
       </c>
       <c r="M3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="N3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4">
@@ -1255,43 +1225,43 @@
         <v>12236.0</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E4" t="n" s="3">
-        <v>36936.2675919213</v>
+        <v>36936.30108271991</v>
       </c>
       <c r="F4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G4" t="n">
         <v>1919.0</v>
       </c>
       <c r="H4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="K4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L4" t="n">
         <v>169754.0</v>
       </c>
       <c r="M4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="N4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5">
@@ -1299,43 +1269,43 @@
         <v>12451.0</v>
       </c>
       <c r="B5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E5" t="n" s="3">
-        <v>31279.267591921296</v>
+        <v>31279.301082719907</v>
       </c>
       <c r="F5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G5" t="n">
         <v>1935.0</v>
       </c>
       <c r="H5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="K5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="L5" t="n">
         <v>233256.0</v>
       </c>
       <c r="M5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="N5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6">
@@ -1343,43 +1313,43 @@
         <v>12781.0</v>
       </c>
       <c r="B6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E6" t="n" s="3">
-        <v>23923.267591921296</v>
+        <v>23923.301082719907</v>
       </c>
       <c r="F6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G6" t="n">
         <v>1955.0</v>
       </c>
       <c r="H6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="I6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="K6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="L6" t="n">
         <v>115897.0</v>
       </c>
       <c r="M6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="N6" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1389,7 +1359,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1403,7 +1373,7 @@
     <col min="6" max="6" width="13.96875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="23.7265625" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="14.23828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="51.51171875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="50.67578125" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="18.09375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="17.89453125" customWidth="true" bestFit="true"/>
@@ -1460,46 +1430,40 @@
         <v>13981.0</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" t="n" s="4">
+        <v>29842.301082719907</v>
+      </c>
+      <c r="F2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" t="s">
         <v>145</v>
       </c>
-      <c r="D2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" t="n" s="4">
-        <v>29842.267591921296</v>
-      </c>
-      <c r="F2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" t="s">
-        <v>144</v>
-      </c>
       <c r="I2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="L2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="M2" t="s">
-        <v>151</v>
-      </c>
-      <c r="N2" t="s">
         <v>152</v>
-      </c>
-      <c r="O2" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="3">
@@ -1507,55 +1471,40 @@
         <v>13657.0</v>
       </c>
       <c r="B3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3" t="s">
         <v>154</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" t="n" s="4">
+        <v>28251.301082719907</v>
+      </c>
+      <c r="F3" t="s">
         <v>155</v>
       </c>
-      <c r="D3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" t="n" s="4">
-        <v>28251.267591921296</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>156</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
+        <v>154</v>
+      </c>
+      <c r="I3" t="s">
         <v>157</v>
       </c>
-      <c r="H3" t="s">
-        <v>155</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>158</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>159</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>160</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>161</v>
-      </c>
-      <c r="M3" t="s">
-        <v>162</v>
-      </c>
-      <c r="N3" t="s">
-        <v>163</v>
-      </c>
-      <c r="O3" t="s">
-        <v>164</v>
-      </c>
-      <c r="P3" t="s">
-        <v>165</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>166</v>
-      </c>
-      <c r="R3" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="4">
@@ -1563,49 +1512,40 @@
         <v>13215.0</v>
       </c>
       <c r="B4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" t="n" s="4">
+        <v>29677.301082719907</v>
+      </c>
+      <c r="F4" t="s">
+        <v>164</v>
+      </c>
+      <c r="G4" t="s">
+        <v>165</v>
+      </c>
+      <c r="H4" t="s">
+        <v>162</v>
+      </c>
+      <c r="I4" t="s">
+        <v>166</v>
+      </c>
+      <c r="J4" t="s">
+        <v>167</v>
+      </c>
+      <c r="K4" t="s">
         <v>168</v>
       </c>
-      <c r="C4" t="s">
+      <c r="L4" t="s">
         <v>169</v>
       </c>
-      <c r="D4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" t="n" s="4">
-        <v>29677.267591921296</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="M4" t="s">
         <v>170</v>
-      </c>
-      <c r="G4" t="s">
-        <v>171</v>
-      </c>
-      <c r="H4" t="s">
-        <v>168</v>
-      </c>
-      <c r="I4" t="s">
-        <v>172</v>
-      </c>
-      <c r="J4" t="s">
-        <v>173</v>
-      </c>
-      <c r="K4" t="s">
-        <v>174</v>
-      </c>
-      <c r="L4" t="s">
-        <v>175</v>
-      </c>
-      <c r="M4" t="s">
-        <v>176</v>
-      </c>
-      <c r="N4" t="s">
-        <v>152</v>
-      </c>
-      <c r="O4" t="s">
-        <v>177</v>
-      </c>
-      <c r="P4" t="s">
-        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1679,13 +1619,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1695,19 +1635,19 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="H2" t="n">
         <v>2.0</v>
       </c>
       <c r="I2" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="J2" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="K2" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="L2" t="n">
         <v>100.0</v>
@@ -1718,37 +1658,37 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C3" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>128</v>
+        <v>174</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="H3" t="n">
         <v>7.0</v>
       </c>
       <c r="I3" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="J3" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="K3" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="L3" t="n">
         <v>100.0</v>
@@ -1759,13 +1699,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B4" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C4" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -1775,19 +1715,19 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="H4" t="n">
         <v>5.0</v>
       </c>
       <c r="I4" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="J4" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="K4" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="L4" t="n">
         <v>100.0</v>
@@ -1867,13 +1807,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B2" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="C2" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1887,7 +1827,7 @@
         <v>2.0</v>
       </c>
       <c r="I2" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="J2" t="n">
         <v>50.0</v>
@@ -1904,13 +1844,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="B3" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="C3" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
@@ -1920,13 +1860,13 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>205</v>
+        <v>174</v>
       </c>
       <c r="H3" t="n">
         <v>2.0</v>
       </c>
       <c r="I3" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="J3" t="n">
         <v>50.0</v>
@@ -1943,13 +1883,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="B4" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="C4" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -1963,7 +1903,7 @@
         <v>2.0</v>
       </c>
       <c r="I4" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="J4" t="n">
         <v>50.0</v>
@@ -2053,31 +1993,31 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>200</v>
       </c>
       <c r="C2" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>136</v>
+        <v>174</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="H2" t="n">
         <v>30.0</v>
       </c>
       <c r="I2" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="J2" t="n">
         <v>250.0</v>
@@ -2086,7 +2026,7 @@
         <v>7.0</v>
       </c>
       <c r="L2" t="s">
-        <v>164</v>
+        <v>200</v>
       </c>
       <c r="M2" t="b">
         <v>1</v>
@@ -2097,31 +2037,31 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C3" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>213</v>
+        <v>174</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>214</v>
+        <v>174</v>
       </c>
       <c r="H3" t="n">
         <v>70.0</v>
       </c>
       <c r="I3" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="J3" t="n">
         <v>250.0</v>
@@ -2130,7 +2070,7 @@
         <v>7.0</v>
       </c>
       <c r="L3" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="M3" t="b">
         <v>1</v>
@@ -2141,13 +2081,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="B4" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="C4" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -2161,7 +2101,7 @@
         <v>40.0</v>
       </c>
       <c r="I4" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="J4" t="n">
         <v>250.0</v>
@@ -2170,7 +2110,7 @@
         <v>7.0</v>
       </c>
       <c r="L4" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="M4" t="b">
         <v>1</v>
@@ -2186,19 +2126,20 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="19.23828125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="17.96484375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="15.9375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="14.5703125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="16.125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="20.58984375" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="12.7421875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="12.6015625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="19.23828125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="17.96484375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="15.9375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="14.5703125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="16.125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="20.58984375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="12.7421875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2223,73 +2164,85 @@
       <c r="G1" t="s" s="1">
         <v>44</v>
       </c>
+      <c r="H1" t="s" s="1">
+        <v>45</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>220</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>221</v>
-      </c>
-      <c r="C2" t="n">
+        <v>210</v>
+      </c>
+      <c r="C2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D2" t="n">
         <v>10.0</v>
       </c>
-      <c r="D2" t="s">
-        <v>180</v>
-      </c>
       <c r="E2" t="s">
-        <v>222</v>
-      </c>
-      <c r="F2" t="n">
+        <v>173</v>
+      </c>
+      <c r="F2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G2" t="n">
         <v>55.18000030517578</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>1275.9000244140625</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>223</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>224</v>
-      </c>
-      <c r="C3" t="n">
+        <v>213</v>
+      </c>
+      <c r="C3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D3" t="n">
         <v>34.0</v>
       </c>
-      <c r="D3" t="s">
-        <v>212</v>
-      </c>
       <c r="E3" t="s">
-        <v>225</v>
-      </c>
-      <c r="F3" t="n">
+        <v>204</v>
+      </c>
+      <c r="F3" t="s">
+        <v>215</v>
+      </c>
+      <c r="G3" t="n">
         <v>15.25</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>8606.75</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>226</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s">
-        <v>227</v>
-      </c>
-      <c r="C4" t="n">
+        <v>216</v>
+      </c>
+      <c r="C4" t="s">
+        <v>217</v>
+      </c>
+      <c r="D4" t="n">
         <v>12.0</v>
       </c>
-      <c r="D4" t="s">
-        <v>204</v>
-      </c>
       <c r="E4" t="s">
-        <v>228</v>
-      </c>
-      <c r="F4" t="n">
+        <v>195</v>
+      </c>
+      <c r="F4" t="s">
+        <v>218</v>
+      </c>
+      <c r="G4" t="n">
         <v>36.7400016784668</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>636.739990234375</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Anmol Singh]Class ExcelWriter-Data Entries attempt 2
</commit_message>
<xml_diff>
--- a/Car_Rental_System.xlsx
+++ b/Car_Rental_System.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="231">
   <si>
     <t>ID</t>
   </si>
@@ -176,7 +176,7 @@
     <t>Me_AnmolSingh</t>
   </si>
   <si>
-    <t>DVLDDVM4L+1jj3a69z/cpAfQlLlVfuUlIkgEvd90w2g=</t>
+    <t>SQCRA1GFP4f9zUI2M4/UUEj1BuCZ4+JGpnGygR8KePM=</t>
   </si>
   <si>
     <t>ghtutgd</t>
@@ -206,7 +206,7 @@
     <t>Me_AmanKaur</t>
   </si>
   <si>
-    <t>6OgKVsE1y+h1P2SVJz0aInXYb1kK5wZkFUZ2eWzwtBM=</t>
+    <t>Y9CLPMIYldDTrs+NcKOZqiVj5H6JgWYIHjZF+YAITQA=</t>
   </si>
   <si>
     <t>458954hgtfr</t>
@@ -233,7 +233,7 @@
     <t>Me_inshant</t>
   </si>
   <si>
-    <t>tqTJTtko45JlgSn9GvNDI6pg7698O6w6NzLyN4b/Alg=</t>
+    <t>UzGh3RBMtT9PCXF4CyC05RnqkUpoGRQdx0BCdiONAgQ=</t>
   </si>
   <si>
     <t>inshant</t>
@@ -257,7 +257,7 @@
     <t>Me_Monica</t>
   </si>
   <si>
-    <t>V40edMd/eJipC7VUDTnNGIkHlumaqe/h1K/jh9MhGUg=</t>
+    <t>DPctE8Ah9gPQQTsJ3ODXIlymCk7Kjgyi1SLJX3QWtm4=</t>
   </si>
   <si>
     <t>5485lkjhy</t>
@@ -284,7 +284,7 @@
     <t>Ikroop_Virk</t>
   </si>
   <si>
-    <t>ZaZkerPOx0xD9w0rwLYgRDV+2mLieQY63rzhVpcGNGg=</t>
+    <t>UTFryGHhxaINpTIhS24Jqf7JopLCk7hz2ZkX9l6/fgo=</t>
   </si>
   <si>
     <t>virkikroop</t>
@@ -305,7 +305,7 @@
     <t>Me_kritima</t>
   </si>
   <si>
-    <t>kGkL2v4KExuxL3+7BRUFyiFUo8t1p0F5xpMR9J7UxOU=</t>
+    <t>btgFIRbg5GCQ3uXItANIV3obtDcDG7bnLysyO4eOypM=</t>
   </si>
   <si>
     <t>5475lkmnj</t>
@@ -320,7 +320,7 @@
     <t>Me_param</t>
   </si>
   <si>
-    <t>LMYaZZ1FON6sEqKJO1o+P/Rly/S/emGVnqtjnfunzfk=</t>
+    <t>0fdYaTzuf/6INmRE4vBvg9D3yW8QgPuMlq2Abs4C0bg=</t>
   </si>
   <si>
     <t>paramkaur</t>
@@ -344,7 +344,7 @@
     <t>KumarShanu</t>
   </si>
   <si>
-    <t>iPYbaG+xNFK4vT73eIlo2HpLgCaNWUS7OhK+QqhyT3Y=</t>
+    <t>FzvIye5Z+oFUgFXsylhodQXDflp8l1nw3p3dYYv5oG4=</t>
   </si>
   <si>
     <t>kjhujh</t>
@@ -371,7 +371,7 @@
     <t>Jordan_Micheal</t>
   </si>
   <si>
-    <t>US5lSqazra80k2WgZYUXWz/cEeH3MOYgtbQeHVhLWSM=</t>
+    <t>d9Q1BkD0Chsfmj4hcaHhgb9g14sHAOTAlFfRzRSpHVo=</t>
   </si>
   <si>
     <t>dfgtre3</t>
@@ -398,7 +398,7 @@
     <t>michelle</t>
   </si>
   <si>
-    <t>EiLI9x3onDSW0W4HLlZqfF6GiSFQs93D4ycCHrQU9/g=</t>
+    <t>vYylz4FFmEJuAQH3ar7v1sS/gBrdTS2l8JFAvi/1r78=</t>
   </si>
   <si>
     <t>1254gytr</t>
@@ -422,7 +422,7 @@
     <t>SherinG</t>
   </si>
   <si>
-    <t>fBNxOejy01MA8AWXJIRhrVZ7FWsBdKskfnXj+MS9n6o=</t>
+    <t>3xo4NAlVAajwZX/SBJCJHT45OLYo3ecrjzzqCZZqcQw=</t>
   </si>
   <si>
     <t>524plo;</t>
@@ -446,7 +446,7 @@
     <t>JainSaab</t>
   </si>
   <si>
-    <t>Th1BuydHm9kvBc0GqTwKTUPvs5vAUmXVM2HWgZuL6ac=</t>
+    <t>DEj2zLq4vr3+qarBWHIlRT0QKn6O676v6Z1Jb6uFZmg=</t>
   </si>
   <si>
     <t>ppo;;lko</t>
@@ -464,7 +464,7 @@
     <t>6723367567</t>
   </si>
   <si>
-    <t>1JVFsnlSA0Xczh9kgiCeDiU5FF50Vdvek7QX+jb2i7g=</t>
+    <t>SQEo4Lf6A1U3RvflW7gMb7/ShDJnSxR9lLDlul7RXPY=</t>
   </si>
   <si>
     <t>ghat</t>
@@ -479,6 +479,12 @@
     <t>auda.org.au</t>
   </si>
   <si>
+    <t>BMX</t>
+  </si>
+  <si>
+    <t>G Wagon</t>
+  </si>
+  <si>
     <t>Gillingum</t>
   </si>
   <si>
@@ -491,7 +497,7 @@
     <t>gillingum@gillingum.com</t>
   </si>
   <si>
-    <t>euiWnjng+cCi5xqyMB8QNkjbS4xJk0fibbRiLBnNRv4=</t>
+    <t>CV9rtBgbOPEyQT9/jD2J9CRY/i5CTA51OxO9kYTLIU4=</t>
   </si>
   <si>
     <t>dhobi_ghat</t>
@@ -506,6 +512,21 @@
     <t>officials.org.au</t>
   </si>
   <si>
+    <t>MINI COACH</t>
+  </si>
+  <si>
+    <t>VOLVO</t>
+  </si>
+  <si>
+    <t>BULLET</t>
+  </si>
+  <si>
+    <t>CIVIC</t>
+  </si>
+  <si>
+    <t>CITY</t>
+  </si>
+  <si>
     <t>Careem</t>
   </si>
   <si>
@@ -518,7 +539,7 @@
     <t>careem@me.com</t>
   </si>
   <si>
-    <t>Vsd/VmktuG3iID8BDPbjwNbm5ZkYPqRBF5fzQH/2bw0=</t>
+    <t>qmLu9i8a2hlGh5eUBfDRBonFw+ZEXYo5r48KFl8hJqY=</t>
   </si>
   <si>
     <t>Gaziattack</t>
@@ -533,6 +554,12 @@
     <t>ComapnyD.org.au</t>
   </si>
   <si>
+    <t>DOUBLE DECKER</t>
+  </si>
+  <si>
+    <t>HARLEY</t>
+  </si>
+  <si>
     <t>JHMZF1C67BS073397</t>
   </si>
   <si>
@@ -542,7 +569,7 @@
     <t>Ford</t>
   </si>
   <si>
-    <t>i</t>
+    <t>IP1</t>
   </si>
   <si>
     <t>Diesel</t>
@@ -563,6 +590,9 @@
     <t>Mercedes</t>
   </si>
   <si>
+    <t>IP5</t>
+  </si>
+  <si>
     <t>Petrol</t>
   </si>
   <si>
@@ -602,12 +632,12 @@
     <t>2HKRL1863YH598774</t>
   </si>
   <si>
-    <t>BMX</t>
-  </si>
-  <si>
     <t>BMW</t>
   </si>
   <si>
+    <t>IP3</t>
+  </si>
+  <si>
     <t>1J4BA6H11AL289387</t>
   </si>
   <si>
@@ -626,6 +656,9 @@
     <t>BusCompany-A</t>
   </si>
   <si>
+    <t>Micheal</t>
+  </si>
+  <si>
     <t>1G1ZT548X5F147693</t>
   </si>
   <si>
@@ -633,6 +666,9 @@
   </si>
   <si>
     <t>BusCompany-B</t>
+  </si>
+  <si>
+    <t>IP4</t>
   </si>
   <si>
     <t>DoubleDecker</t>
@@ -749,7 +785,7 @@
     <col min="6" max="6" width="13.96875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="20.828125" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="15.8203125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="50.96875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="52.6328125" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="12.28125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="10.59375" customWidth="true" bestFit="true"/>
@@ -807,7 +843,7 @@
         <v>48</v>
       </c>
       <c r="E2" t="n" s="2">
-        <v>35749.30108271991</v>
+        <v>35749.3036696875</v>
       </c>
       <c r="F2" t="s">
         <v>49</v>
@@ -845,7 +881,7 @@
         <v>58</v>
       </c>
       <c r="E3" t="n" s="2">
-        <v>35637.30108271991</v>
+        <v>35637.3036696875</v>
       </c>
       <c r="F3" t="s">
         <v>59</v>
@@ -883,7 +919,7 @@
         <v>48</v>
       </c>
       <c r="E4" t="n" s="2">
-        <v>35445.30108271991</v>
+        <v>35445.3036696875</v>
       </c>
       <c r="F4" t="s">
         <v>68</v>
@@ -921,7 +957,7 @@
         <v>58</v>
       </c>
       <c r="E5" t="n" s="2">
-        <v>35602.30108271991</v>
+        <v>35602.3036696875</v>
       </c>
       <c r="F5" t="s">
         <v>76</v>
@@ -959,7 +995,7 @@
         <v>58</v>
       </c>
       <c r="E6" t="n" s="2">
-        <v>34912.30108271991</v>
+        <v>34912.3036696875</v>
       </c>
       <c r="F6" t="s">
         <v>85</v>
@@ -997,7 +1033,7 @@
         <v>58</v>
       </c>
       <c r="E7" t="n" s="2">
-        <v>35567.30108271991</v>
+        <v>35567.3036696875</v>
       </c>
       <c r="F7" t="s">
         <v>92</v>
@@ -1035,7 +1071,7 @@
         <v>58</v>
       </c>
       <c r="E8" t="n" s="2">
-        <v>33783.30108271991</v>
+        <v>33783.3036696875</v>
       </c>
       <c r="F8" t="s">
         <v>92</v>
@@ -1081,7 +1117,7 @@
     <col min="7" max="7" width="5.77734375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="21.96875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="15.25" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="53.7734375" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="49.859375" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="20.04296875" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="18.6328125" customWidth="true" bestFit="true"/>
@@ -1146,7 +1182,7 @@
         <v>48</v>
       </c>
       <c r="E2" t="n" s="3">
-        <v>35735.30108271991</v>
+        <v>35735.3036696875</v>
       </c>
       <c r="F2" t="s">
         <v>105</v>
@@ -1190,7 +1226,7 @@
         <v>48</v>
       </c>
       <c r="E3" t="n" s="3">
-        <v>28476.301082719907</v>
+        <v>28476.3036696875</v>
       </c>
       <c r="F3" t="s">
         <v>114</v>
@@ -1234,7 +1270,7 @@
         <v>58</v>
       </c>
       <c r="E4" t="n" s="3">
-        <v>36936.30108271991</v>
+        <v>36936.3036696875</v>
       </c>
       <c r="F4" t="s">
         <v>123</v>
@@ -1278,7 +1314,7 @@
         <v>58</v>
       </c>
       <c r="E5" t="n" s="3">
-        <v>31279.301082719907</v>
+        <v>31279.3036696875</v>
       </c>
       <c r="F5" t="s">
         <v>131</v>
@@ -1322,7 +1358,7 @@
         <v>48</v>
       </c>
       <c r="E6" t="n" s="3">
-        <v>23923.301082719907</v>
+        <v>23923.3036696875</v>
       </c>
       <c r="F6" t="s">
         <v>139</v>
@@ -1359,7 +1395,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1373,12 +1409,12 @@
     <col min="6" max="6" width="13.96875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="23.7265625" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="14.23828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="50.67578125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="48.9140625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="18.09375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="17.89453125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="17.125" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="14.45703125" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="15.96484375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1439,7 +1475,7 @@
         <v>58</v>
       </c>
       <c r="E2" t="n" s="4">
-        <v>29842.301082719907</v>
+        <v>29842.3036696875</v>
       </c>
       <c r="F2" t="s">
         <v>147</v>
@@ -1464,6 +1500,12 @@
       </c>
       <c r="M2" t="s">
         <v>152</v>
+      </c>
+      <c r="N2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O2" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="3">
@@ -1471,40 +1513,55 @@
         <v>13657.0</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C3" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D3" t="s">
         <v>48</v>
       </c>
       <c r="E3" t="n" s="4">
-        <v>28251.301082719907</v>
+        <v>28251.3036696875</v>
       </c>
       <c r="F3" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="G3" t="s">
+        <v>158</v>
+      </c>
+      <c r="H3" t="s">
         <v>156</v>
       </c>
-      <c r="H3" t="s">
-        <v>154</v>
-      </c>
       <c r="I3" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="J3" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="K3" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="L3" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="M3" t="s">
-        <v>161</v>
+        <v>163</v>
+      </c>
+      <c r="N3" t="s">
+        <v>164</v>
+      </c>
+      <c r="O3" t="s">
+        <v>165</v>
+      </c>
+      <c r="P3" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>167</v>
+      </c>
+      <c r="R3" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="4">
@@ -1512,40 +1569,49 @@
         <v>13215.0</v>
       </c>
       <c r="B4" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="C4" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="D4" t="s">
         <v>58</v>
       </c>
       <c r="E4" t="n" s="4">
-        <v>29677.301082719907</v>
+        <v>29677.3036696875</v>
       </c>
       <c r="F4" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="G4" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="H4" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="I4" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="J4" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="K4" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="L4" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="M4" t="s">
-        <v>170</v>
+        <v>177</v>
+      </c>
+      <c r="N4" t="s">
+        <v>178</v>
+      </c>
+      <c r="O4" t="s">
+        <v>179</v>
+      </c>
+      <c r="P4" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -1619,13 +1685,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="B2" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="C2" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1635,19 +1701,19 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="H2" t="n">
         <v>2.0</v>
       </c>
       <c r="I2" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="J2" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="K2" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="L2" t="n">
         <v>100.0</v>
@@ -1658,37 +1724,37 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="B3" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="C3" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>174</v>
+        <v>129</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="H3" t="n">
         <v>7.0</v>
       </c>
       <c r="I3" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="J3" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="K3" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="L3" t="n">
         <v>100.0</v>
@@ -1699,13 +1765,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="B4" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="C4" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -1715,19 +1781,19 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="H4" t="n">
         <v>5.0</v>
       </c>
       <c r="I4" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="J4" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="K4" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="L4" t="n">
         <v>100.0</v>
@@ -1807,13 +1873,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="B2" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="C2" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1827,7 +1893,7 @@
         <v>2.0</v>
       </c>
       <c r="I2" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="J2" t="n">
         <v>50.0</v>
@@ -1844,13 +1910,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="B3" t="s">
-        <v>194</v>
+        <v>153</v>
       </c>
       <c r="C3" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
@@ -1860,13 +1926,13 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>174</v>
+        <v>205</v>
       </c>
       <c r="H3" t="n">
         <v>2.0</v>
       </c>
       <c r="I3" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="J3" t="n">
         <v>50.0</v>
@@ -1883,13 +1949,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="B4" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="C4" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -1903,7 +1969,7 @@
         <v>2.0</v>
       </c>
       <c r="I4" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="J4" t="n">
         <v>50.0</v>
@@ -1935,7 +2001,7 @@
     <col min="2" max="2" width="23.8125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="25.03515625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="13.63671875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="8.51953125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="8.70703125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="11.921875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="30.76171875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="15.09375" customWidth="true" bestFit="true"/>
@@ -1993,31 +2059,31 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="B2" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="C2" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>174</v>
+        <v>205</v>
       </c>
       <c r="H2" t="n">
         <v>30.0</v>
       </c>
       <c r="I2" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="J2" t="n">
         <v>250.0</v>
@@ -2026,7 +2092,7 @@
         <v>7.0</v>
       </c>
       <c r="L2" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="M2" t="b">
         <v>1</v>
@@ -2037,31 +2103,31 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="B3" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="C3" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>174</v>
+        <v>121</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>174</v>
+        <v>216</v>
       </c>
       <c r="H3" t="n">
         <v>70.0</v>
       </c>
       <c r="I3" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="J3" t="n">
         <v>250.0</v>
@@ -2070,7 +2136,7 @@
         <v>7.0</v>
       </c>
       <c r="L3" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="M3" t="b">
         <v>1</v>
@@ -2081,13 +2147,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="B4" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="C4" t="s">
-        <v>208</v>
+        <v>220</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -2101,7 +2167,7 @@
         <v>40.0</v>
       </c>
       <c r="I4" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="J4" t="n">
         <v>250.0</v>
@@ -2110,7 +2176,7 @@
         <v>7.0</v>
       </c>
       <c r="L4" t="s">
-        <v>209</v>
+        <v>221</v>
       </c>
       <c r="M4" t="b">
         <v>1</v>
@@ -2173,19 +2239,19 @@
         <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="C2" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="D2" t="n">
         <v>10.0</v>
       </c>
       <c r="E2" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="F2" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="G2" t="n">
         <v>55.18000030517578</v>
@@ -2199,19 +2265,19 @@
         <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>213</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="D3" t="n">
         <v>34.0</v>
       </c>
       <c r="E3" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="F3" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="G3" t="n">
         <v>15.25</v>
@@ -2225,19 +2291,19 @@
         <v>90</v>
       </c>
       <c r="B4" t="s">
-        <v>216</v>
+        <v>228</v>
       </c>
       <c r="C4" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="D4" t="n">
         <v>12.0</v>
       </c>
       <c r="E4" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="F4" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="G4" t="n">
         <v>36.7400016784668</v>

</xml_diff>